<commit_message>
Update readme and spreadsheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\school\intro-research\bluebikes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\school\intro-research\bluebikes-angel-navigator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652E38F-E74B-41F8-BC36-9CCE2EC5FE40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFDCD43-E00B-4A07-A11A-F98B43911104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Ratio of bikes to total docks</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Actual points</t>
+  </si>
+  <si>
+    <t>Distr</t>
+  </si>
+  <si>
+    <t>Val</t>
   </si>
 </sst>
 </file>
@@ -2983,7 +2989,360 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>data!$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$36:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDC9-44C7-8789-FBD65A02049F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="603289520"/>
+        <c:axId val="603288688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="603289520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603288688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="603288688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603289520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3520,6 +3879,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4357,6 +5219,42 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>36443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>115956</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>112643</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF83E054-1EFD-4064-BEA4-7969AF69FEC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4450,20 +5348,20 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1391 1184 12552 0 0,'0'0'598'0'0,"-2"-2"-103"0"0,2 2-300 0 0,-2-2-426 0 0,-2-11 4591 0 0,4 13-4296 0 0,-5 16 429 0 0,-4 24-384 0 0,-21 172 535 0 0,25-46-348 0 0,5-84-162 0 0,5 119 204 0 0,-1-91-40 0 0,-2 61 400 0 0,-2-171-692 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-9-5 156 0 0,1-1-147 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,1-2 0 0 0,-9-12 0 0 0,8 8 33 0 0,0 0 0 0 0,1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,-4-25 0 0 0,5 13 7 0 0,3 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,2 2 0 0 0,1-1 0 0 0,1-1 0 0 0,4-28 1 0 0,0 25-22 0 0,1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,1 2 0 0 0,1 0-1 0 0,2 0 1 0 0,1 0 0 0 0,1 3 0 0 0,1-1 0 0 0,21-28 0 0 0,-15 28 17 0 0,1 3 1 0 0,35-30-1 0 0,-20 20 3 0 0,-31 27-44 0 0,10-8 38 0 0,30-23 0 0 0,-41 33-42 0 0,-1 2 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,9 0 0 0 0,-7 1 4 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,11 6 0 0 0,-15-6-4 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-2-1 0 0,0 1 1 0 0,0 0 0 0 0,2 5 0 0 0,-1-1 3 0 0,0 2 1 0 0,0-1 0 0 0,-2-1 0 0 0,1 2-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,-1 9 0 0 0,-3 4 14 0 0,-1-1 1 0 0,-11 35-1 0 0,0-17 33 0 0,-1 1 1 0 0,-3-3-1 0 0,-27 40 0 0 0,27-42-30 0 0,-13 20 115 0 0,30-52-125 0 0,3-6 18 0 0,4-9 28 0 0,10-4-354 0 0,21-21 1 0 0,-26 29-2024 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="401.06">2366 1104 13768 0 0,'-1'5'65'0'0,"1"0"1"0"0,-1-1 0 0 0,0 2-1 0 0,0-2 1 0 0,0 0 0 0 0,-3 6 0 0 0,-1 2 146 0 0,-70 238 1748 0 0,34-106-1374 0 0,39-136-554 0 0,0-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-2 1 0 0,1 10-1 0 0,0-13-2 0 0,-1-1 0 0 0,1 2 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,5 2 0 0 0,0-1 15 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,9-3 0 0 0,-1 1 53 0 0,-1-1 1 0 0,0-1 0 0 0,21-11-1 0 0,-23 8-38 0 0,0 2-1 0 0,-1-3 0 0 0,0 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,0-2-1 0 0,0 0 1 0 0,-1 1-1 0 0,-1-2 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-2 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 0-1 0 0,6-25 1 0 0,-7 24-4 0 0,-2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0 1 0 0 0,-5-21 0 0 0,7 35-45 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,-4 0-1 0 0,2 0 18 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,-6 4 0 0 0,0-2 52 0 0,1 2-1 0 0,-12 6 0 0 0,19-9-59 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 1 0 0,1 0-1 0 0,-3 6 0 0 0,4-9-12 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 2-1 0 0,1-2 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1-1 0 0,0 1 13 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,3 0 0 0 0,11-4 133 0 0,0-1 0 0 0,26-12 0 0 0,-11 3-3233 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="744.13">2847 1299 13672 0 0,'3'40'536'0'0,"-1"-1"0"0"0,-3 0 0 0 0,-7 71 0 0 0,3-2 903 0 0,5-99-1360 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,5 11 0 0 0,-7-20-71 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,5-10 242 0 0,28-72 464 0 0,-17 33-3469 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1150.97">2988 954 16072 0 0,'0'0'869'0'0,"0"1"-666"0"0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,2 2-116 0 0,1-1 1 0 0,0 0 0 0 0,0 1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,2 6 1 0 0,-4-8-9 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,0-1 0 0 0,8 5-2738 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1488.12">3232 1470 14872 0 0,'1'38'407'0'0,"-3"1"0"0"0,-1 0 0 0 0,-7 41-1 0 0,-55 210 1758 0 0,65-290-2164 0 0,-1 4 3 0 0,-1 6 127 0 0,-1 1 1 0 0,-7 18-1 0 0,10-28 75 0 0,1-17-21 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,1 0-1 0 0,7-20 0 0 0,-2 4 22 0 0,-1 6-140 0 0,1 1 1 0 0,0 0 0 0 0,2 1 0 0 0,0-1 0 0 0,23-32-1 0 0,-6 16 52 0 0,2 2 0 0 0,34-36 0 0 0,-46 55-93 0 0,40-41 134 0 0,-47 52-133 0 0,-1 0 0 0 0,1 1 0 0 0,24-14 0 0 0,-33 21-24 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-3 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 5 0 0 0,4 11 0 0 0,0 1 0 0 0,-1-1 0 0 0,7 39 0 0 0,-7-19 0 0 0,2 42 0 0 0,-7-27 4 0 0,-1-32-3 0 0,1 1-1 0 0,5 34 1 0 0,-1-30 15 0 0,1-2 0 0 0,0 1 0 0 0,17 44 0 0 0,-22-69-16 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-2 0 0 0,-1 2-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-2 0 0 0,4-2 31 0 0,-1 0 1 0 0,1-2-1 0 0,6-8 1 0 0,-10 12-26 0 0,15-22 37 0 0,-2-2 0 0 0,-1 0 0 0 0,17-45 1 0 0,-14 32 27 0 0,36-80-12 0 0,77-207 134 0 0,-90 197-214 0 0,43-136-51 0 0,-75 245-12 0 0,0 0 0 0 0,0 1 0 0 0,3 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,15-18 1 0 0,-10 23-426 0 0,-14 12 498 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,2 9-46 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 8 0 0 0,-9 55-531 0 0,6-52 515 0 0,-47 262-147 0 0,13-89 126 0 0,30-155 109 0 0,-25 203 236 0 0,31-237-149 0 0,1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 4-1 0 0,-2-7-79 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 2 1 0 0,0-2 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,12-6-2686 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1836.78">4378 1404 15176 0 0,'-10'-32'208'0'0,"7"21"-42"0"0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-7-9 0 0 0,2 7 151 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,-13-10 0 0 0,16 15-215 0 0,1 1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-15-3 0 0 0,5 4-31 0 0,2 1 1 0 0,-2 0-1 0 0,1 2 1 0 0,0 0 0 0 0,0 0-1 0 0,0 3 1 0 0,0-1-1 0 0,-16 6 1 0 0,10 1 41 0 0,0 1-1 0 0,-23 14 1 0 0,-10 6 43 0 0,47-28-93 0 0,7-3-47 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 2-1 0 0,0-2 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,2-2 6 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,3 1 0 0 0,-1 1 21 0 0,17 6 6 0 0,-1-1-1 0 0,1 0 1 0 0,24 2-1 0 0,-3-1-2726 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2164.64">4350 1357 12360 0 0,'11'-4'18'0'0,"1"0"0"0"0,19-3-1 0 0,0 0 19 0 0,-24 5 120 0 0,-1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,7-8 1 0 0,-11 9 106 0 0,-7 4 225 0 0,-6 3 194 0 0,9-3-624 0 0,0 0 0 0 0,1 0 1 0 0,-1 2-1 0 0,0-2 0 0 0,0 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 2 1 0 0,0-2 65 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 2 0 0 0,2-2-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,3 4 1 0 0,2 3 49 0 0,1-2 0 0 0,0 1 0 0 0,0-2 0 0 0,1 1 1 0 0,17 13-1 0 0,-16-13 49 0 0,1-1 1 0 0,-1 2-1 0 0,15 17 1 0 0,-23-23-177 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 1 0 0,1 10-1 0 0,-1-5 11 0 0,0 0 1 0 0,-1-1-1 0 0,-1 1 1 0 0,0-2-1 0 0,0 2 1 0 0,-1-2-1 0 0,1 2 1 0 0,-6 9-1 0 0,-4 9 121 0 0,-17 29 0 0 0,4-14 1 0 0,-1-3 0 0 0,-38 45 0 0 0,62-83-164 0 0,-1 2 23 0 0,0-1-1 0 0,1 0 1 0 0,-1 2 0 0 0,-1-2 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-7 2-1 0 0,9-5-33 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1-9 154 0 0,9-14 116 0 0,-7 22-265 0 0,71-170 360 0 0,-47 119-159 0 0,37-59 0 0 0,-10 28-425 0 0,-35 56-2558 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168703.78">3845 3474 12552 0 0,'0'0'0'0'0,"3"-2"0"0"0,1-2 0 0 0,2-3 40 0 0,3-2-8 0 0,1 0-32 0 0,3 3 0 0 0,9-3 112 0 0,1-4-8 0 0,-1 2-104 0 0,-2-1 0 0 0,-2 1-8 0 0,-1 1 8 0 0,-1-4 0 0 0,-1-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168702.78">4772 2543 12552 0 0,'32'-22'480'0'0,"-2"-4"0"0"0,37-37 0 0 0,48-69 326 0 0,-82 92-2488 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168372.36">5610 1588 12056 0 0,'0'0'0'0'0,"4"-4"0"0"0,4-6 0 0 0,3-1-16 0 0,4-2 8 0 0,1 1 8 0 0,1 1 0 0 0,2 3 72 0 0,-3 1 0 0 0,0-2-72 0 0,1-2 0 0 0,-2-1 24 0 0,-2 2-8 0 0,1-3-16 0 0,0-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167815.49">6171 958 10952 0 0,'-1'-16'598'0'0,"1"12"-256"0"0,-1 1 1 0 0,1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1-1 1 0 0,1 1 0 0 0,1 1-1 0 0,-2-1 1 0 0,4-6 0 0 0,0 4-307 0 0,0-2 1 0 0,-1 0-1 0 0,5-12 1 0 0,-6 12-2 0 0,2-2 0 0 0,5-9 0 0 0,-8 17-35 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-4 0 0 0,0 6-4 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-4 0-17 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,-3 2 0 0 0,2 0-8 0 0,-4 1-6 0 0,-2 1-1 0 0,2 0 1 0 0,1 2 0 0 0,-1-1 0 0 0,1 2-1 0 0,-1-1 1 0 0,-12 16 0 0 0,-18 11-54 0 0,-107 76-149 0 0,105-79 161 0 0,27-21 61 0 0,0-2 1 0 0,-1 0-1 0 0,2-1 1 0 0,-26 7-1 0 0,22-8 14 0 0,-19 13-28 0 0,17-9 23 0 0,3 3-20 0 0,8-6 20 0 0,9-7 5 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 2 0 0 0,0-2-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,9-3 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,11-7 0 0 0,6-4 0 0 0,56-32-1 0 0,128-88 3 0 0,-193 125-1 0 0,15-10 3 0 0,31-20 0 0 0,-53 37-3 0 0,0 0-1 0 0,0 0 1 0 0,1 2-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,16-2 0 0 0,-21 4 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,7 3-1 0 0,-9-3 1 0 0,0-1 1 0 0,1 2-1 0 0,-1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2 1 0 0,0 1-1 0 0,0 3 11 0 0,0 2 0 0 0,0-1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,-3 13 0 0 0,-3 9 83 0 0,-13 29 1 0 0,13-39-82 0 0,-91 237 770 0 0,77-194-690 0 0,1-1-767 0 0,-29 60 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-165393.82">1 649 15472 0 0,'1'6'165'0'0,"0"0"1"0"0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,5 11 0 0 0,-1-1 234 0 0,10 26 421 0 0,1-3 0 0 0,2 0-1 0 0,31 46 1 0 0,5 2-268 0 0,47 98 1 0 0,-79-133-390 0 0,-2 0 1 0 0,-2 1 0 0 0,24 91-1 0 0,15 210 415 0 0,-54-313-485 0 0,2-2-1 0 0,16 56 1 0 0,-19-81-69 0 0,1 0 0 0 0,0-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-1-3 0 0 0,1 2 0 0 0,1-1 0 0 0,13 12 0 0 0,33 23 115 0 0,-34-30-3113 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-165059.59">1246 1313 16072 0 0,'-54'109'214'0'0,"18"-39"-55"0"0,-113 289 199 0 0,18-40-162 0 0,-137 232 331 0 0,126-239-331 0 0,19 9 88 0 0,83-199-124 0 0,26-76-2465 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-164141.43">6732 160 14464 0 0,'-2'-22'66'0'0,"2"9"466"0"0,0 13-516 0 0,-1-2-1 0 0,1 2 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 43 0 0,4-4 410 0 0,45-20 138 0 0,-17 9-427 0 0,0 2-1 0 0,2 2 0 0 0,38-9 0 0 0,-19 11 146 0 0,69-3-1 0 0,-112 11-229 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,17 6 0 0 0,-26-8-71 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 2 0 0 0,0 3 26 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,-1 9-1 0 0,2-10 43 0 0,-8 19-4 0 0,0 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,-19 30 0 0 0,12-21-49 0 0,-29 51 101 0 0,-48 104 383 0 0,84-162-459 0 0,2-1 1 0 0,0 2-1 0 0,1 0 0 0 0,-7 53 0 0 0,14-74-39 0 0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 2 1 0 0,1-2-1 0 0,1 0 0 0 0,-1 1 1 0 0,2-2-1 0 0,-1 2 1 0 0,0-1-1 0 0,6 12 0 0 0,-5-14-7 0 0,-1-1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 1 0 0 0,1-2 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-2 0 0 0,1 1 0 0 0,-2 1 0 0 0,2-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,5 1 0 0 0,0-2 29 0 0,0 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0-1-1 0 0,14-5 1 0 0,64-35 170 0 0,-86 42-203 0 0,23-15 22 0 0,1 0-1 0 0,-1-2 1 0 0,29-28 0 0 0,63-71 140 0 0,-91 88-158 0 0,48-55 164 0 0,-49 53-2547 0 0,-22 28 1773 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1402 1184 12552 0 0,'0'0'598'0'0,"-2"-2"-103"0"0,2 2-300 0 0,-2-2-426 0 0,-2-11 4591 0 0,4 13-4296 0 0,-5 16 429 0 0,-4 24-384 0 0,-21 172 535 0 0,25-46-348 0 0,5-84-162 0 0,5 119 204 0 0,-1-91-40 0 0,-2 61 400 0 0,-2-171-692 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-9-5 156 0 0,1-1-147 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,2-1 0 0 0,0 1 0 0 0,1-2 0 0 0,-9-12 0 0 0,8 8 33 0 0,0 0 0 0 0,1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,-4-25 0 0 0,5 13 7 0 0,3 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,2 2 0 0 0,1-1 0 0 0,1-1 0 0 0,4-28 1 0 0,0 25-22 0 0,1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,1 2 0 0 0,1 0-1 0 0,2 0 1 0 0,1 0 0 0 0,2 3 0 0 0,0-1 0 0 0,21-28 0 0 0,-15 28 17 0 0,1 3 1 0 0,36-30-1 0 0,-21 20 3 0 0,-31 27-44 0 0,10-8 38 0 0,31-23 0 0 0,-42 33-42 0 0,-1 2 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,9 0 0 0 0,-7 1 4 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,11 6 0 0 0,-15-6-4 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-2-1 0 0,0 1 1 0 0,0 0 0 0 0,2 5 0 0 0,-1-1 3 0 0,0 2 1 0 0,0-1 0 0 0,-2-1 0 0 0,1 2-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,-1 9 0 0 0,-3 4 14 0 0,-1-1 1 0 0,-11 35-1 0 0,0-17 33 0 0,-1 1 1 0 0,-3-3-1 0 0,-28 40 0 0 0,28-42-30 0 0,-13 20 115 0 0,30-52-125 0 0,3-6 18 0 0,4-9 28 0 0,10-4-354 0 0,21-21 1 0 0,-26 29-2024 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="401.06">2385 1104 13768 0 0,'-1'5'65'0'0,"1"0"1"0"0,-1-1 0 0 0,0 2-1 0 0,0-2 1 0 0,0 0 0 0 0,-3 6 0 0 0,-1 2 146 0 0,-70 238 1748 0 0,33-106-1374 0 0,40-136-554 0 0,0-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-2 1 0 0,1 10-1 0 0,0-13-2 0 0,-1-1 0 0 0,1 2 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,5 2 0 0 0,1-1 15 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,9-3 0 0 0,-1 1 53 0 0,-1-1 1 0 0,1-1 0 0 0,20-11-1 0 0,-23 8-38 0 0,0 2-1 0 0,-1-3 0 0 0,0 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1-2-1 0 0,-1 0 1 0 0,-1 1-1 0 0,-1-2 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-2 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 0-1 0 0,6-25 1 0 0,-7 24-4 0 0,-2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0 1 0 0 0,-5-21 0 0 0,7 35-45 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,-4 0-1 0 0,2 0 18 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,-6 4 0 0 0,0-2 52 0 0,1 2-1 0 0,-13 6 0 0 0,20-9-59 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 1 0 0,1 0-1 0 0,-3 6 0 0 0,4-9-12 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 2-1 0 0,1-2 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1-1 0 0,0 1 13 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,3 0 0 0 0,11-4 133 0 0,1-1 0 0 0,25-12 0 0 0,-11 3-3233 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="744.13">2870 1299 13672 0 0,'3'40'536'0'0,"-1"-1"0"0"0,-3 0 0 0 0,-7 71 0 0 0,3-2 903 0 0,5-99-1360 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,5 11 0 0 0,-7-20-71 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,5-10 242 0 0,29-72 464 0 0,-18 33-3469 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1150.97">3012 954 16072 0 0,'0'0'869'0'0,"0"1"-666"0"0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,2 2-116 0 0,1-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,2 6 1 0 0,-4-8-9 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,0-1 0 0 0,8 5-2738 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1488.12">3258 1470 14872 0 0,'1'38'407'0'0,"-3"1"0"0"0,-1 0 0 0 0,-7 41-1 0 0,-55 210 1758 0 0,65-290-2164 0 0,-1 4 3 0 0,-1 6 127 0 0,-1 1 1 0 0,-7 18-1 0 0,10-28 75 0 0,1-17-21 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,1 0-1 0 0,7-20 0 0 0,-2 4 22 0 0,-1 6-140 0 0,1 1 1 0 0,0 0 0 0 0,2 1 0 0 0,0-1 0 0 0,23-32-1 0 0,-5 16 52 0 0,1 2 0 0 0,34-36 0 0 0,-45 55-93 0 0,39-41 134 0 0,-47 52-133 0 0,-1 0 0 0 0,1 1 0 0 0,25-14 0 0 0,-34 21-24 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-3 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 5 0 0 0,4 11 0 0 0,0 1 0 0 0,-1-1 0 0 0,8 39 0 0 0,-8-19 0 0 0,2 42 0 0 0,-7-27 4 0 0,-1-32-3 0 0,1 1-1 0 0,5 34 1 0 0,-1-30 15 0 0,1-2 0 0 0,0 1 0 0 0,17 44 0 0 0,-22-69-16 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-2 0 0 0,-1 2-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-2 0 0 0,4-2 31 0 0,-1 0 1 0 0,1-2-1 0 0,6-8 1 0 0,-10 12-26 0 0,16-22 37 0 0,-3-2 0 0 0,-1 0 0 0 0,17-45 1 0 0,-14 32 27 0 0,37-80-12 0 0,77-207 134 0 0,-91 197-214 0 0,44-136-51 0 0,-76 245-12 0 0,0 0 0 0 0,0 1 0 0 0,3 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,15-18 1 0 0,-10 23-426 0 0,-14 12 498 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,2 9-46 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 8 0 0 0,-9 55-531 0 0,6-52 515 0 0,-47 262-147 0 0,13-89 126 0 0,30-155 109 0 0,-26 203 236 0 0,32-237-149 0 0,1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 4-1 0 0,-2-7-79 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 2 1 0 0,0-2 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,12-6-2686 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1836.78">4414 1404 15176 0 0,'-10'-32'208'0'0,"7"21"-42"0"0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-7-9 0 0 0,2 7 151 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,-13-10 0 0 0,16 15-215 0 0,1 1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-15-3 0 0 0,5 4-31 0 0,2 1 1 0 0,-2 0-1 0 0,1 2 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 3 1 0 0,0-1-1 0 0,-16 6 1 0 0,10 1 41 0 0,0 1-1 0 0,-24 14 1 0 0,-9 6 43 0 0,47-28-93 0 0,7-3-47 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 2-1 0 0,0-2 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,2-2 6 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,3 1 0 0 0,-1 1 21 0 0,17 6 6 0 0,-1-1-1 0 0,1 0 1 0 0,24 2-1 0 0,-2-1-2726 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2164.64">4385 1357 12360 0 0,'12'-4'18'0'0,"0"0"0"0"0,19-3-1 0 0,0 0 19 0 0,-24 5 120 0 0,-1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,7-8 1 0 0,-11 9 106 0 0,-7 4 225 0 0,-6 3 194 0 0,9-3-624 0 0,0 0 0 0 0,1 0 1 0 0,-1 2-1 0 0,0-2 0 0 0,0 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 2 1 0 0,0-2 65 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 2 0 0 0,2-2-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,4 4 1 0 0,1 3 49 0 0,1-2 0 0 0,0 1 0 0 0,0-2 0 0 0,1 1 1 0 0,17 13-1 0 0,-16-13 49 0 0,1-1 1 0 0,-1 2-1 0 0,16 17 1 0 0,-24-23-177 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 1 0 0,1 10-1 0 0,-1-5 11 0 0,0 0 1 0 0,-1-1-1 0 0,-1 1 1 0 0,0-2-1 0 0,0 2 1 0 0,-1-2-1 0 0,1 2 1 0 0,-6 9-1 0 0,-5 9 121 0 0,-16 29 0 0 0,4-14 1 0 0,-1-3 0 0 0,-39 45 0 0 0,63-83-164 0 0,-1 2 23 0 0,0-1-1 0 0,1 0 1 0 0,-1 2 0 0 0,-1-2 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-7 2-1 0 0,9-5-33 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1-9 154 0 0,9-14 116 0 0,-7 22-265 0 0,72-170 360 0 0,-48 119-159 0 0,37-59 0 0 0,-9 28-425 0 0,-36 56-2558 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168703.78">3876 3474 12552 0 0,'0'0'0'0'0,"3"-2"0"0"0,1-2 0 0 0,2-3 40 0 0,3-2-8 0 0,2 0-32 0 0,2 3 0 0 0,9-3 112 0 0,1-4-8 0 0,-1 2-104 0 0,-2-1 0 0 0,-1 1-8 0 0,-2 1 8 0 0,-1-4 0 0 0,-1-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168702.78">4811 2543 12552 0 0,'32'-22'480'0'0,"-2"-4"0"0"0,38-37 0 0 0,48-69 326 0 0,-83 92-2488 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168372.36">5656 1588 12056 0 0,'0'0'0'0'0,"4"-4"0"0"0,4-6 0 0 0,3-1-16 0 0,4-2 8 0 0,1 1 8 0 0,1 1 0 0 0,2 3 72 0 0,-2 1 0 0 0,-1-2-72 0 0,1-2 0 0 0,-2-1 24 0 0,-2 2-8 0 0,1-3-16 0 0,0-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167815.49">6221 958 10952 0 0,'-1'-16'598'0'0,"1"12"-256"0"0,-1 1 1 0 0,1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1-1 1 0 0,1 1 0 0 0,1 1-1 0 0,-2-1 1 0 0,4-6 0 0 0,0 4-307 0 0,0-2 1 0 0,-1 0-1 0 0,5-12 1 0 0,-6 12-2 0 0,3-2 0 0 0,4-9 0 0 0,-8 17-35 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-4 0 0 0,0 6-4 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-5 0-17 0 0,2 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,-3 2 0 0 0,2 0-8 0 0,-4 1-6 0 0,-2 1-1 0 0,2 0 1 0 0,1 2 0 0 0,-1-1 0 0 0,1 2-1 0 0,-1-1 1 0 0,-12 16 0 0 0,-19 11-54 0 0,-107 76-149 0 0,106-79 161 0 0,27-21 61 0 0,-1-2 1 0 0,0 0-1 0 0,2-1 1 0 0,-26 7-1 0 0,22-8 14 0 0,-20 13-28 0 0,18-9 23 0 0,3 3-20 0 0,8-6 20 0 0,9-7 5 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 2 0 0 0,0-2-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,9-3 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,12-7 0 0 0,5-4 0 0 0,56-32-1 0 0,130-88 3 0 0,-195 125-1 0 0,16-10 3 0 0,30-20 0 0 0,-53 37-3 0 0,0 0-1 0 0,0 0 1 0 0,1 2-1 0 0,0 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,16-2 0 0 0,-21 4 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,7 3-1 0 0,-9-3 1 0 0,0-1 1 0 0,1 2-1 0 0,-1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2 1 0 0,0 1-1 0 0,0 3 11 0 0,0 2 0 0 0,0-1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,-4 13 0 0 0,-2 9 83 0 0,-13 29 1 0 0,13-39-82 0 0,-92 237 770 0 0,78-194-690 0 0,1-1-767 0 0,-29 60 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-165393.82">1 649 15472 0 0,'1'6'165'0'0,"0"0"1"0"0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,5 11 0 0 0,-1-1 234 0 0,10 26 421 0 0,1-3 0 0 0,3 0-1 0 0,30 46 1 0 0,6 2-268 0 0,46 98 1 0 0,-78-133-390 0 0,-3 0 1 0 0,-2 1 0 0 0,24 91-1 0 0,16 210 415 0 0,-55-313-485 0 0,2-2-1 0 0,16 56 1 0 0,-19-81-69 0 0,1 0 0 0 0,0-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-1-3 0 0 0,1 2 0 0 0,2-1 0 0 0,12 12 0 0 0,33 23 115 0 0,-34-30-3113 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-165059.59">1256 1313 16072 0 0,'-54'109'214'0'0,"17"-39"-55"0"0,-113 289 199 0 0,18-40-162 0 0,-138 232 331 0 0,127-239-331 0 0,19 9 88 0 0,83-199-124 0 0,27-76-2465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-164141.43">6787 160 14464 0 0,'-2'-22'66'0'0,"2"9"466"0"0,0 13-516 0 0,-1-2-1 0 0,1 2 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 43 0 0,4-4 410 0 0,45-20 138 0 0,-16 9-427 0 0,-1 2-1 0 0,2 2 0 0 0,39-9 0 0 0,-20 11 146 0 0,70-3-1 0 0,-113 11-229 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,17 6 0 0 0,-26-8-71 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 2 0 0 0,0 3 26 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,-1 9-1 0 0,2-10 43 0 0,-8 19-4 0 0,0 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,-20 30 0 0 0,13-21-49 0 0,-29 51 101 0 0,-49 104 383 0 0,85-162-459 0 0,2-1 1 0 0,0 2-1 0 0,1 0 0 0 0,-7 53 0 0 0,14-74-39 0 0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 2 1 0 0,1-2-1 0 0,1 0 0 0 0,-1 1 1 0 0,2-2-1 0 0,-1 2 1 0 0,0-1-1 0 0,6 12 0 0 0,-5-14-7 0 0,-1-1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 1 0 0 0,1-2 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-2 0 0 0,1 1 0 0 0,-2 1 0 0 0,2-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,5 1 0 0 0,1-2 29 0 0,-1 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0-1-1 0 0,14-5 1 0 0,65-35 170 0 0,-87 42-203 0 0,23-15 22 0 0,1 0-1 0 0,0-2 1 0 0,28-28 0 0 0,64-71 140 0 0,-92 88-158 0 0,49-55 164 0 0,-50 53-2547 0 0,-22 28 1773 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4494,20 +5392,20 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2930 3354 11760 0 0,'0'0'490'0'0,"0"-7"3309"0"0,1-1-3594 0 0,0 4-172 0 0,-1 3-22 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,14-16 129 0 0,8-11 22 0 0,41-38 0 0 0,-57 59-159 0 0,155-145 394 0 0,-92 75-54 0 0,-43 48-2727 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="346.18">3846 2388 11952 0 0,'6'-7'233'0'0,"0"0"1"0"0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,2 0-1 0 0,-2 0 1 0 0,14-3-1 0 0,-18 6-199 0 0,-1-1-1 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,2-5 0 0 0,8-5 128 0 0,2-5-42 0 0,-1-1 1 0 0,0 0 0 0 0,16-28-1 0 0,-5 9-8 0 0,10-15-1968 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22624.31">7118 1200 7632 0 0,'0'0'56'0'0,"-19"36"-56"0"0,15-21-168 0 0,-1-1 168 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23267.64">6353 5983 14872 0 0,'0'0'1104'0'0,"-3"21"-473"0"0,3-19-7 0 0,3-2-608 0 0,4 0 16 0 0,15-27-32 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23601.03">8064 2485 14776 0 0,'1'0'53'0'0,"0"0"0"0"0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,19 13 785 0 0,-16-13-784 0 0,-1 1-53 0 0,8 15 342 0 0,-7-10-2466 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23939.14">7496 5754 15376 0 0,'-12'41'175'0'0,"8"-33"-131"0"0,1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,2 1 1 0 0,-3 15-1 0 0,3-21-33 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-1 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,1 0-1 0 0,1-1 9 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,6-4-1 0 0,4-4 96 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,17-21-1 0 0,-16 18-1333 0 0,18-32 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24616.62">8373 5914 14968 0 0,'0'0'0'0'0,"-2"-6"0"0"0,2 2 0 0 0,-2-3 264 0 0,0-4 8 0 0,4-8-272 0 0,6-9 0 0 0,7-9 8 0 0,4-5 0 0 0,4-10-8 0 0,-2-12 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24277.78">10154 1009 16072 0 0,'12'-8'-8'0'0,"5"-6"-74"0"0,1 1-1 0 0,1 1 1 0 0,22-11-1 0 0,-35 20 70 0 0,-2 1-1 0 0,2 0 1 0 0,1 0-1 0 0,-2 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 2-1 0 0,0 0 1 0 0,0-1 0 0 0,7 4-1 0 0,-10-4 36 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 2 0 0 0,-1-2-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 7-1 0 0,0 0 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-2 0 1 0 0,-2 13 0 0 0,-36 83-1812 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24278.78">10082 5874 15576 0 0,'0'0'0'0'0,"-5"30"0"0"0,3 1-32 0 0,0 11 8 0 0,4-3 24 0 0,5-5 0 0 0,8-7 16 0 0,1-6 0 0 0,2-7-16 0 0,1-7 0 0 0,-3-7 0 0 0,0-5 0 0 0,-5-7 0 0 0,-1 1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24949">10051 1384 14672 0 0,'0'0'0'0'0,"5"1"0"0"0,10 2-48 0 0,15-3 48 0 0,-1 0-336 0 0,4 0 16 0 0,3-3 320 0 0,3-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24950">11994 595 14968 0 0,'0'0'0'0'0,"-2"7"0"0"0,-2 4 0 0 0,-1 7 24 0 0,0 3-8 0 0,-3 11-16 0 0,-3 5 0 0 0,-1 12 16 0 0,-2 6 8 0 0,-5 10-24 0 0,-4 9 0 0 0,-7 14-184 0 0,-4 7 0 0 0,-6 9 184 0 0,-8 7 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38050.43">273 5727 13360 0 0,'0'0'729'0'0,"-4"1"-117"0"0,-1 0-500 0 0,-13 1 1041 0 0,17-2-1124 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,-1-3 525 0 0,-2-20 79 0 0,1-10-495 0 0,1 0-1 0 0,1 0 1 0 0,2 0 0 0 0,1 0 0 0 0,2 0 0 0 0,12-52 0 0 0,12-34 11 0 0,15-52 89 0 0,-13 73-30 0 0,81-177 1 0 0,42-91-18 0 0,-61 131 9 0 0,311-726 215 0 0,-334 784-348 0 0,-32 79-47 0 0,-14 32-9 0 0,-10 28 17 0 0,24-50-1 0 0,-33 78-25 0 0,1 0 1 0 0,-1 1-1 0 0,2 0 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,12-10-1 0 0,-1 6 5 0 0,0 0 0 0 0,1 2-1 0 0,37-14 1 0 0,-39 17-7 0 0,-2 2 2 0 0,0-1-1 0 0,27-2 1 0 0,-27 6 0 0 0,0-2 0 0 0,31-9 1 0 0,-8-3 6 0 0,1 1 1 0 0,0 4 0 0 0,44-7-1 0 0,9 6 23 0 0,72-9 13 0 0,25-2-12 0 0,1 16 12 0 0,-92 4-38 0 0,47-9 20 0 0,-19 1-9 0 0,118-21 14 0 0,-2-22-15 0 0,-89 18-1 0 0,149-44 13 0 0,-33 8-2 0 0,371-73 40 0 0,-435 98-26 0 0,388-93 20 0 0,85-52-4 0 0,-140 37 13 0 0,2 16-36 0 0,-534 137-35 0 0,797-190 54 0 0,-338 92-19 0 0,-151 35-9 0 0,-197 38-9 0 0,309-69 22 0 0,-2-17 10 0 0,-265 64-41 0 0,351-113 39 0 0,-60 19 14 0 0,-276 98-39 0 0,104-27 26 0 0,-102 30-32 0 0,-7 1 4 0 0,-81 14-6 0 0,85-24 5 0 0,4 14 17 0 0,-73 18-16 0 0,44-4 4 0 0,-139 21-17 0 0,2 2 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 1 0 0 0,12 4 0 0 0,-18-5-4 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,6 7 1 0 0,-8-6 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 8 0 0 0,4 6 9 0 0,-4-11-10 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,-3 19 1 0 0,-3 5 15 0 0,-20 64 0 0 0,10-44-13 0 0,-14 64 3 0 0,12-42 4 0 0,-29 79 0 0 0,-83 193 26 0 0,35-109-20 0 0,-3 9 4 0 0,-48 217 54 0 0,30-28-20 0 0,13-50-12 0 0,38-107-32 0 0,-16 64 4 0 0,7 6-3 0 0,69-312-12 0 0,-34 175 0 0 0,25-146-2 0 0,-25 73 1 0 0,34-118 0 0 0,4-15 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-5 9 0 0 0,6-14 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-5-2 0 0 0,-8-5 0 0 0,3 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 3 0 0 0,0-1 0 0 0,-1 2 0 0 0,-22-3 0 0 0,-124 1-8 0 0,91 7 4 0 0,14 1 0 0 0,-174 13-10 0 0,0 20-13 0 0,-46 6 6 0 0,-308 12-5 0 0,-207 27 26 0 0,237 14 0 0 0,432-71 0 0 0,-118 28-1 0 0,-120 21-4 0 0,-694 117-37 0 0,935-167 36 0 0,-376 54-13 0 0,68-12 3 0 0,-11-1-4 0 0,-184-7 8 0 0,47-13-3 0 0,405-36 12 0 0,-140 12-10 0 0,-388 100-48 0 0,284-30 5 0 0,383-83 57 0 0,-224 33-41 0 0,169-29 14 0 0,-417 38-78 0 0,380-36 44 0 0,1 7 1 0 0,-136 41-1 0 0,-153 74-83 0 0,327-103 122 0 0,-34 17-50 0 0,96-38 58 0 0,2 0 0 0 0,-1 2-1 0 0,-24 19 1 0 0,16-4-17 0 0,21-20 20 0 0,0 1 0 0 0,-1-2-1 0 0,1 1 1 0 0,-12 5 0 0 0,9-6-17 0 0,-17 14 0 0 0,21-16-15 0 0,15-11 17 0 0,1 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,10-17 1 0 0,24-39-143 0 0,-28 39 148 0 0,1 0-2686 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38376.04">306 5593 11656 0 0,'-12'50'6'0'0,"-15"79"38"0"0,1 36 204 0 0,5-37 207 0 0,-8 149 0 0 0,27-239-2065 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39105.93">331 5160 11856 0 0,'-6'14'1'0'0,"-21"58"204"0"0,2 3 58 0 0,5-7-54 0 0,-28 122 513 0 0,35-102-475 0 0,-6 25 184 0 0,18-107-857 0 0,0 2-1 0 0,0-1 0 0 0,0 9 1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2965 3354 11760 0 0,'0'0'490'0'0,"0"-7"3309"0"0,1-1-3594 0 0,0 4-172 0 0,-1 3-22 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,14-16 129 0 0,9-11 22 0 0,40-38 0 0 0,-57 59-159 0 0,157-145 394 0 0,-93 75-54 0 0,-43 48-2727 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="346.18">3892 2388 11952 0 0,'6'-7'233'0'0,"0"0"1"0"0,0 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,2 1 1 0 0,-2 1 0 0 0,2 0-1 0 0,-2 0 1 0 0,14-3-1 0 0,-18 6-199 0 0,-1-1-1 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,2-5 0 0 0,9-5 128 0 0,1-5-42 0 0,-1-1 1 0 0,0 0 0 0 0,16-28-1 0 0,-4 9-8 0 0,9-15-1968 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22624.31">7203 1200 7632 0 0,'0'0'56'0'0,"-19"36"-56"0"0,15-21-168 0 0,-1-1 168 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23267.64">6429 5983 14872 0 0,'0'0'1104'0'0,"-3"21"-473"0"0,3-19-7 0 0,3-2-608 0 0,4 0 16 0 0,15-27-32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23601.03">8160 2485 14776 0 0,'1'0'53'0'0,"0"0"0"0"0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,20 13 785 0 0,-17-13-784 0 0,-1 1-53 0 0,8 15 342 0 0,-7-10-2466 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23939.14">7585 5754 15376 0 0,'-12'41'175'0'0,"8"-33"-131"0"0,1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,2 1 1 0 0,-3 15-1 0 0,3-21-33 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-1 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,1 0-1 0 0,1-1 9 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,6-4-1 0 0,4-4 96 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1-1 0 0 0,17-21-1 0 0,-16 18-1333 0 0,19-32 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24616.62">8473 5914 14968 0 0,'0'0'0'0'0,"-2"-6"0"0"0,2 2 0 0 0,-2-3 264 0 0,0-4 8 0 0,4-8-272 0 0,6-9 0 0 0,7-9 8 0 0,4-5 0 0 0,5-10-8 0 0,-3-12 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24277.78">10275 1009 16072 0 0,'12'-8'-8'0'0,"5"-6"-74"0"0,2 1-1 0 0,0 1 1 0 0,22-11-1 0 0,-35 20 70 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,-2 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 2-1 0 0,0 0 1 0 0,1-1 0 0 0,6 4-1 0 0,-10-4 36 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 2 0 0 0,-1-2-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 7-1 0 0,0 0 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-2 0 1 0 0,-2 13 0 0 0,-36 83-1812 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24278.78">10202 5874 15576 0 0,'0'0'0'0'0,"-5"30"0"0"0,3 1-32 0 0,0 11 8 0 0,4-3 24 0 0,5-5 0 0 0,8-7 16 0 0,2-6 0 0 0,1-7-16 0 0,1-7 0 0 0,-3-7 0 0 0,0-5 0 0 0,-4-7 0 0 0,-2 1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24949">10171 1384 14672 0 0,'0'0'0'0'0,"5"1"0"0"0,10 2-48 0 0,15-3 48 0 0,0 0-336 0 0,3 0 16 0 0,4-3 320 0 0,2-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24950">12137 595 14968 0 0,'0'0'0'0'0,"-2"7"0"0"0,-2 4 0 0 0,-1 7 24 0 0,0 3-8 0 0,-3 11-16 0 0,-3 5 0 0 0,-1 12 16 0 0,-3 6 8 0 0,-4 10-24 0 0,-4 9 0 0 0,-8 14-184 0 0,-3 7 0 0 0,-6 9 184 0 0,-9 7 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38050.43">276 5727 13360 0 0,'0'0'729'0'0,"-4"1"-117"0"0,-1 0-500 0 0,-13 1 1041 0 0,17-2-1124 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,-1-3 525 0 0,-2-20 79 0 0,1-10-495 0 0,1 0-1 0 0,1 0 1 0 0,2 0 0 0 0,1 0 0 0 0,2 0 0 0 0,12-52 0 0 0,12-34 11 0 0,16-52 89 0 0,-14 73-30 0 0,83-177 1 0 0,41-91-18 0 0,-60 131 9 0 0,313-726 215 0 0,-337 784-348 0 0,-32 79-47 0 0,-15 32-9 0 0,-10 28 17 0 0,25-50-1 0 0,-34 78-25 0 0,1 0 1 0 0,-1 1-1 0 0,2 0 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,13-10-1 0 0,-2 6 5 0 0,0 0 0 0 0,1 2-1 0 0,38-14 1 0 0,-40 17-7 0 0,-2 2 2 0 0,1-1-1 0 0,26-2 1 0 0,-27 6 0 0 0,0-2 0 0 0,32-9 1 0 0,-9-3 6 0 0,2 1 1 0 0,-1 4 0 0 0,45-7-1 0 0,9 6 23 0 0,73-9 13 0 0,26-2-12 0 0,0 16 12 0 0,-93 4-38 0 0,48-9 20 0 0,-20 1-9 0 0,120-21 14 0 0,-2-22-15 0 0,-90 18-1 0 0,151-44 13 0 0,-34 8-2 0 0,376-73 40 0 0,-441 98-26 0 0,393-93 20 0 0,86-52-4 0 0,-141 37 13 0 0,1 16-36 0 0,-540 137-35 0 0,807-190 54 0 0,-343 92-19 0 0,-152 35-9 0 0,-199 38-9 0 0,312-69 22 0 0,-2-17 10 0 0,-268 64-41 0 0,355-113 39 0 0,-61 19 14 0 0,-279 98-39 0 0,105-27 26 0 0,-102 30-32 0 0,-8 1 4 0 0,-82 14-6 0 0,86-24 5 0 0,4 14 17 0 0,-74 18-16 0 0,45-4 4 0 0,-141 21-17 0 0,2 2 0 0 0,-2-1 1 0 0,0 1-1 0 0,2 1 0 0 0,11 4 0 0 0,-18-5-4 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,7 7 1 0 0,-9-6 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 8 0 0 0,4 6 9 0 0,-4-11-10 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,-3 19 1 0 0,-3 5 15 0 0,-20 64 0 0 0,9-44-13 0 0,-13 64 3 0 0,12-42 4 0 0,-30 79 0 0 0,-83 193 26 0 0,34-109-20 0 0,-2 9 4 0 0,-48 217 54 0 0,29-28-20 0 0,14-50-12 0 0,38-107-32 0 0,-16 64 4 0 0,7 6-3 0 0,70-312-12 0 0,-34 175 0 0 0,24-146-2 0 0,-24 73 1 0 0,34-118 0 0 0,4-15 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-5 9 0 0 0,6-14 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-5-2 0 0 0,-8-5 0 0 0,3 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 3 0 0 0,0-1 0 0 0,-1 2 0 0 0,-23-3 0 0 0,-125 1-8 0 0,93 7 4 0 0,13 1 0 0 0,-176 13-10 0 0,0 20-13 0 0,-46 6 6 0 0,-312 12-5 0 0,-209 27 26 0 0,239 14 0 0 0,438-71 0 0 0,-120 28-1 0 0,-122 21-4 0 0,-701 117-37 0 0,945-167 36 0 0,-379 54-13 0 0,67-12 3 0 0,-10-1-4 0 0,-186-7 8 0 0,47-13-3 0 0,410-36 12 0 0,-142 12-10 0 0,-392 100-48 0 0,287-30 5 0 0,387-83 57 0 0,-226 33-41 0 0,171-29 14 0 0,-422 38-78 0 0,385-36 44 0 0,0 7 1 0 0,-137 41-1 0 0,-155 74-83 0 0,331-103 122 0 0,-34 17-50 0 0,97-38 58 0 0,1 0 0 0 0,0 2-1 0 0,-24 19 1 0 0,15-4-17 0 0,22-20 20 0 0,0 1 0 0 0,-1-2-1 0 0,1 1 1 0 0,-12 5 0 0 0,8-6-17 0 0,-16 14 0 0 0,21-16-15 0 0,15-11 17 0 0,1 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,11-17 1 0 0,23-39-143 0 0,-28 39 148 0 0,1 0-2686 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38376.04">310 5593 11656 0 0,'-12'50'6'0'0,"-16"79"38"0"0,2 36 204 0 0,5-37 207 0 0,-9 149 0 0 0,28-239-2065 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39105.93">335 5160 11856 0 0,'-6'14'1'0'0,"-21"58"204"0"0,1 3 58 0 0,6-7-54 0 0,-29 122 513 0 0,36-102-475 0 0,-6 25 184 0 0,18-107-857 0 0,0 2-1 0 0,0-1 0 0 0,0 9 1 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4541,8 +5439,8 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">9 363 14968 0 0,'1'21'391'0'0,"3"24"1"0"0,2 14 731 0 0,-9 87 115 0 0,1-29-655 0 0,6 94 49 0 0,-5-196-573 0 0,1-2 0 0 0,-2 2 0 0 0,-3 23 0 0 0,3-34 61 0 0,1-5-49 0 0,-3-10-28 0 0,0-16-22 0 0,4 6-6 0 0,1-1-1 0 0,5-35 1 0 0,-2 31-2 0 0,1-14 6 0 0,2-1 0 0 0,3 1-1 0 0,0 0 1 0 0,2 0 0 0 0,2 2-1 0 0,20-40 1 0 0,-27 62-5 0 0,1 1 0 0 0,2 2-1 0 0,-2-2 1 0 0,3 2 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 2-1 0 0,2-1 1 0 0,-1 2 0 0 0,1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,1 2 0 0 0,17-7 0 0 0,-24 11 8 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,15 3 1 0 0,62 19 199 0 0,-66-17-209 0 0,6 4 54 0 0,-14-4 73 0 0,21 3 0 0 0,-28-7-119 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,5-2 1 0 0,10-2-219 0 0,-14 4-2232 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="516.77">1152 290 14568 0 0,'4'1'301'0'0,"5"4"1048"0"0,-9-5-1327 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,-29 28 1580 0 0,-111 92-965 0 0,110-91-443 0 0,2 2 0 0 0,-37 49-1 0 0,50-56-59 0 0,1 2 0 0 0,0 1 0 0 0,2-1 0 0 0,1 1 0 0 0,1 1 0 0 0,1 1 0 0 0,-8 37 0 0 0,17-60-88 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1-1 0 0,3 13 1 0 0,-3-17-24 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 2-1 0 0,-1-1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1-1 0 0,18 6 215 0 0,-11-6-207 0 0,1 0-1 0 0,-2-1 1 0 0,2 0 0 0 0,0-1 0 0 0,-2 0-1 0 0,13-5 1 0 0,-14 4-20 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,5-12 0 0 0,4-8 49 0 0,22-48-1 0 0,-35 70-57 0 0,58-157 180 0 0,-6 14-49 0 0,-36 89 86 0 0,-17 73 10 0 0,0-6-222 0 0,-4 56 116 0 0,3 79-1 0 0,2-62-62 0 0,-1-78-56 0 0,0 21 37 0 0,4 30 0 0 0,-4-48-33 0 0,2 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,0-1-1 0 0,8 16 0 0 0,-9-18-4 0 0,1 1 13 0 0,1-2 0 0 0,-1 1 0 0 0,8 10 0 0 0,-10-15-15 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,2-1 0 0 0,6-4 12 0 0,0 0 0 0 0,-2-1 0 0 0,2-1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,12-16 0 0 0,2-6-3077 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="869.58">1668 95 14464 0 0,'5'-9'82'0'0,"1"1"0"0"0,-1-2 0 0 0,4-11 1 0 0,-5 13 51 0 0,0-2 0 0 0,1 2 1 0 0,7-13-1 0 0,-12 21-116 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 11 754 0 0,-23 42-514 0 0,0 0 23 0 0,-11 55-7 0 0,-10 25 265 0 0,21-70 100 0 0,3 2 0 0 0,2 0-1 0 0,-11 68 1 0 0,28-113-397 0 0,0 1-1 0 0,1 0 1 0 0,2 23 0 0 0,-1-42-223 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-2-1 1 0 0,4-1-1 0 0,10-6 53 0 0,-1-1 0 0 0,14-11-1 0 0,-10 5-2994 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1200.88">1825 515 13560 0 0,'1'-3'27'0'0,"0"1"1"0"0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 10 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 2-1 0 0,-4-4 1 0 0,-2 0 69 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 3 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-10 1-1 0 0,-85 25 173 0 0,-15 4 434 0 0,109-29-565 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-13 9 0 0 0,22-13-84 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-2 1-1 0 0,2-2-38 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,11 6-2557 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1201.88">2042 475 15576 0 0,'3'3'43'0'0,"-2"-2"-30"0"0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1 7 77 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,-3 14-1 0 0,0 7 241 0 0,0-2 0 0 0,-3 1 1 0 0,-16 48-1 0 0,-13 24 85 0 0,36-99-380 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-2 3 0 0 0,4-5-13 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-2 0 0 0,1 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1-14 126 0 0,1 14-43 0 0,6-133 302 0 0,2 82-3052 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1200.86">1825 515 13560 0 0,'1'-3'27'0'0,"0"1"1"0"0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 10 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 2-1 0 0,-4-4 1 0 0,-2 0 69 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 3 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-10 1-1 0 0,-85 25 173 0 0,-15 4 434 0 0,109-29-565 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-13 9 0 0 0,22-13-84 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-2 1-1 0 0,2-2-38 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,11 6-2557 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1201.86">2042 475 15576 0 0,'3'3'43'0'0,"-2"-2"-30"0"0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1 7 77 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,-3 14-1 0 0,0 7 241 0 0,0-2 0 0 0,-3 1 1 0 0,-16 48-1 0 0,-13 24 85 0 0,36-99-380 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-2 3 0 0 0,4-5-13 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-2 0 0 0,1 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1-14 126 0 0,1 14-43 0 0,6-133 302 0 0,2 82-3052 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1598.71">2100 380 12664 0 0,'0'0'0'0'0,"2"-3"0"0"0,3 0 0 0 0,-1-1 24 0 0,-3-2 8 0 0,4 1-32 0 0,-1-1 0 0 0,-1-2 16 0 0,1-2 8 0 0,3-1-24 0 0,3-4 0 0 0,2-3-8 0 0,1 1 8 0 0,-3-1 0 0 0,1 1 0 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1930.83">2332 439 13560 0 0,'-11'38'78'0'0,"9"-30"-15"0"0,0 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,-3 11 1 0 0,-31 40 1098 0 0,26-42-719 0 0,1-1-1 0 0,0 2 0 0 0,-9 20 0 0 0,6-6-327 0 0,7-19 21 0 0,1 1 0 0 0,1-2-1 0 0,0 2 1 0 0,-6 27 0 0 0,10-40-118 0 0,-1 3 121 0 0,0 1 0 0 0,1-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,1 10 0 0 0,-1-11-71 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,2 0 1 0 0,0-1-1 0 0,0 2 0 0 0,0-2 1 0 0,4 4-1 0 0,3 2 92 0 0,2 2 0 0 0,0-2 0 0 0,22 13 0 0 0,-26-17-80 0 0,-2-2 0 0 0,2 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1-1 0 0 0,11 1-1 0 0,-8-2 4 0 0,1 0-1 0 0,15-2 0 0 0,-23 2-65 0 0,1-1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,4-4-1 0 0,0-1 6 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-2 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-13 0 0 0,-1-5 33 0 0,-2 2 0 0 0,-7-40-1 0 0,9 57-37 0 0,-2 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 2-1 0 0,-2-1 0 0 0,0 0 1 0 0,0 2-1 0 0,-7-10 0 0 0,7 12 14 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-8 0 1 0 0,-5 1 95 0 0,-1 1 0 0 0,1 1 0 0 0,-27 6 0 0 0,-47 5 214 0 0,92-13-330 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 1 0 0,-2-6-3088 0 0</inkml:trace>
 </inkml:ink>
@@ -4578,7 +5476,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">153 98 15680 0 0,'0'0'682'0'0,"-1"5"-105"0"0,-5 95 1551 0 0,4-26-1357 0 0,1-71-734 0 0,-6 107 621 0 0,-22 114 0 0 0,14-142-570 0 0,2-11 48 0 0,-22 74 0 0 0,33-135-115 0 0,-3 0 0 0 0,0 1 0 0 0,-7 11 0 0 0,1-1-1 0 0,5-2 32 0 0,4-12-16 0 0,3-9-18 0 0,8-11-3 0 0,-3 5-8 0 0,33-60 4 0 0,-29 49-5 0 0,0 1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 2 0 0 0,26-28 0 0 0,-30 37-3 0 0,0-1 0 0 0,1 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,2 1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,19-5-1 0 0,-22 8 0 0 0,1-1 1 0 0,0 1 0 0 0,-2 1 0 0 0,2-1-1 0 0,9 2 1 0 0,-14 0 2 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,4 4 0 0 0,-7-5-4 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 2-1 0 0,-2 4 13 0 0,1 0 0 0 0,-1-1 0 0 0,-4 8 0 0 0,4-9-14 0 0,-9 22 27 0 0,-1-1 0 0 0,-2 0 0 0 0,1-1-1 0 0,-26 32 1 0 0,24-38 26 0 0,-29 26 0 0 0,27-28-5 0 0,-21 26-1 0 0,27-29-4 0 0,0-1 0 0 0,-2-1 0 0 0,1 1-1 0 0,-2-2 1 0 0,-27 19 0 0 0,34-27 129 0 0,7-3-89 0 0,2-7-4 0 0,6-9 275 0 0,16-30-1 0 0,0 10-3831 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="333.83">754 755 16575 0 0,'-2'2'22'0'0,"0"0"64"0"0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 5 1 0 0,-6 28 138 0 0,5-17 201 0 0,-3 7-211 0 0,-2-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-2 0 0 0,-15 27-1 0 0,19-39-108 0 0,0-1 81 0 0,3-9-116 0 0,0-7-43 0 0,1 0-2502 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="749.87">1360 1 17383 0 0,'-1'1'-42'0'0,"1"1"0"0"0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 1-1 0 0,-2 10-154 0 0,-46 109 273 0 0,19-41 409 0 0,4 2-1 0 0,-31 170 1 0 0,51-204 20 0 0,0 65 0 0 0,6-98-282 0 0,1 50 225 0 0,2 2 0 0 0,15 80 0 0 0,-17-141-361 0 0,7 38 444 0 0,-7-42-497 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,3 3 0 0 0,-5-7-13 0 0,0 2-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-2 1 0 0,-1 2-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0 1 0 0,8-16-2075 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1096.1">1589 447 16384 0 0,'-72'41'207'0'0,"-30"13"377"0"0,2-1 61 0 0,87-44-509 0 0,-1 0 1 0 0,1 1-1 0 0,1 1 1 0 0,-22 22-1 0 0,29-28-86 0 0,1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-2-1 0 0,1 9 1 0 0,0-12-25 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,3 3 1 0 0,18 15 565 0 0,-19-18-523 0 0,3 5 28 0 0,1-3 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,12 5-1 0 0,-1-2 130 0 0,26 4 0 0 0,-36-9-143 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,13-3 0 0 0,6-5 281 0 0,32-15 1 0 0,-45 18-238 0 0,-1 0 1 0 0,0-3 0 0 0,1 1 0 0 0,13-13-1 0 0,-20 15-481 0 0,-1 0-1 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1-2 0 0 0,1 2 0 0 0,8-17 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1096.08">1589 447 16384 0 0,'-72'41'207'0'0,"-30"13"377"0"0,2-1 61 0 0,87-44-509 0 0,-1 0 1 0 0,1 1-1 0 0,1 1 1 0 0,-22 22-1 0 0,29-28-86 0 0,1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-2-1 0 0,1 9 1 0 0,0-12-25 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,3 3 1 0 0,18 15 565 0 0,-19-18-523 0 0,3 5 28 0 0,1-3 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,12 5-1 0 0,-1-2 130 0 0,26 4 0 0 0,-36-9-143 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,13-3 0 0 0,6-5 281 0 0,32-15 1 0 0,-45 18-238 0 0,-1 0 1 0 0,0-3 0 0 0,1 1 0 0 0,13-13-1 0 0,-20 15-481 0 0,-1 0-1 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1-2 0 0 0,1 2 0 0 0,8-17 0 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1430.48">1862 812 15472 0 0,'18'17'90'0'0,"1"0"1"0"0,20 15 0 0 0,-36-31-68 0 0,0 1 1 0 0,0 1 0 0 0,-1-2 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,6 1 1 0 0,-3-2 66 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,7-6 0 0 0,-2 2 15 0 0,-1-1-1 0 0,0 0 0 0 0,1-2 0 0 0,-2 1 1 0 0,0 0-1 0 0,11-13 0 0 0,-9 8-24 0 0,0-1-1 0 0,-2 0 1 0 0,1-1 0 0 0,-1-1 0 0 0,-2 1-1 0 0,1-2 1 0 0,10-28 0 0 0,-14 33 33 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0-2-1 0 0,-1 1 0 0 0,0-1 0 0 0,-1 2 1 0 0,-3-12-1 0 0,4 19-82 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,-2-2 0 0 0,1 2 5 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-5 0 0 0 0,-2 1 13 0 0,-1 1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 3-1 0 0,0-2 1 0 0,-1 1 0 0 0,2 0-1 0 0,0 2 1 0 0,-10 9 0 0 0,-7 9 117 0 0,1 2 0 0 0,2 1 0 0 0,-20 33 0 0 0,25-36-84 0 0,1 2 0 0 0,-14 32-1 0 0,23-44-40 0 0,1 1-1 0 0,0-1 0 0 0,2 1 1 0 0,0 0-1 0 0,-4 26 0 0 0,8-42-33 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 3 0 0 0,-1-4 2 0 0,0 1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,1 0 0 0 0,6 0 60 0 0,-4 0-57 0 0,-1 1-1 0 0,2-1 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,1 0 0 0 0,0-2-1 0 0,0 2 1 0 0,0-1 0 0 0,5-4-1 0 0,22-15 14 0 0,42-38 0 0 0,-42 34-2818 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1860.12">2608 491 16384 0 0,'0'1'34'0'0,"0"1"52"0"0,-1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-3 2 0 0 0,-2 6 140 0 0,-16 25 232 0 0,-3-1 0 0 0,0 1-1 0 0,-2-3 1 0 0,-35 32-1 0 0,50-51-432 0 0,-32 33 294 0 0,38-40-251 0 0,1 1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-5 11 1 0 0,8-15-2 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 1 0 0,1 5-1 0 0,0 0 11 0 0,1 0 1 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,7 9 1 0 0,-1-2 253 0 0,15 15 1 0 0,-14-16-239 0 0,17 24 0 0 0,-23-32 19 0 0,4 8 61 0 0,-1-1 1 0 0,11 27-1 0 0,-16-35-139 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-2 7 1 0 0,-4 5 21 0 0,0 1 1 0 0,-1-1 0 0 0,0-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,-18 22 0 0 0,-2-2 154 0 0,-44 37 1 0 0,64-63-174 0 0,1 1-1 0 0,-1-2 0 0 0,-1-1 1 0 0,-18 11-1 0 0,22-14-22 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-17-1 0 0 0,20-1-7 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-2-1 0 0,1 2 1 0 0,0-1-1 0 0,0 1 0 0 0,-3-5 1 0 0,3 3 3 0 0,1 1-1 0 0,0-2 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,1-5 0 0 0,12-38-1582 0 0,-13 43-50 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2217.32">3033 588 17887 0 0,'-52'79'48'0'0,"19"-26"42"0"0,-170 272 1004 0 0,105-172-785 0 0,15-27-10 0 0,11-3 6 0 0,-15 22-2 0 0,73-125-82 0 0,-17 21 0 0 0,1-5 55 0 0,28-34-212 0 0,2-3 488 0 0,3-5-3434 0 0</inkml:trace>
@@ -4782,18 +5680,18 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">235 246 15072 0 0,'-15'1'143'0'0,"0"1"0"0"0,1 0 1 0 0,0 2-1 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 3 0 0 0,-13 8 1 0 0,22-14-88 0 0,0 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 2-1 0 0,0-2 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 9 0 0 0,3-4-16 0 0,0-1 1 0 0,0-1 0 0 0,1 2-1 0 0,-1-2 1 0 0,2 2 0 0 0,-1-1 0 0 0,1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,6 10 1 0 0,42 99 343 0 0,8 17 43 0 0,-32-78-346 0 0,66 126 612 0 0,-82-163-620 0 0,8 12 168 0 0,-1 2 0 0 0,24 56 0 0 0,-40-83-216 0 0,1 0 0 0 0,-2 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0-1-1 0 0,-1 2 1 0 0,0-1-1 0 0,0-1 1 0 0,0 1-1 0 0,-5 8 1 0 0,3-7 18 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-2-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,-8 3 1 0 0,-1-2 12 0 0,0 0-1 0 0,0-2 1 0 0,0 1 0 0 0,0-2 0 0 0,0 0 0 0 0,0-2 0 0 0,0 0-1 0 0,-16-4 1 0 0,16 1 14 0 0,0 0-1 0 0,-1-1 0 0 0,-26-15 1 0 0,40 19-63 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 2 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2-5-1 0 0,2 3 15 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-6 0 0 0,2-1 26 0 0,0-2 0 0 0,0 2 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,9-11 0 0 0,64-88 135 0 0,-53 80-81 0 0,-3-1 0 0 0,32-56-1 0 0,63-180 275 0 0,-95 216-321 0 0,-7 17 58 0 0,-4 11-38 0 0,0-1 0 0 0,6-28 0 0 0,-14 46-40 0 0,0-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-3-10 0 0 0,3 15-17 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 2 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,-4 0 66 0 0,-2-1 0 0 0,-10-1 0 0 0,-77-10 178 0 0,94 14-271 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-3 1 0 0 0,-5 3-2848 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="334.59">837 695 18991 0 0,'5'5'1256'0'0,"7"-8"1220"0"0,-10 0-2284 0 0,-2 3-174 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1-2-1 0 0,-1 2 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,0-3 37 0 0,-5-4 173 0 0,6 8-223 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2 0 0 0,-1-2 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-4 6-2996 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="662.14">724 1268 15472 0 0,'0'0'0'0'0,"0"-2"0"0"0,0 0 0 0 0,0 0 216 0 0,0-1 8 0 0,0 1-224 0 0,0-1 0 0 0,0-1 264 0 0,0-2-9 0 0,0-7-255 0 0,0-8 0 0 0,0-9 0 0 0,0-6 0 0 0,0 1 0 0 0,0 3 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1000.97">1273 408 15072 0 0,'14'-6'141'0'0,"17"-3"0"0"0,-20 7 46 0 0,-1-1 0 0 0,0-2 0 0 0,16-5 0 0 0,-20 6-6 0 0,1 0 0 0 0,0 0 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,15-1 0 0 0,-19 2-157 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 2-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 2-1 0 0,0-2 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,2 2 1 0 0,-1-2-1 0 0,0 1 1 0 0,0-1-1 0 0,1 5 0 0 0,-1-3-10 0 0,0 2-1 0 0,0-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-2 1 0 0,-1 0-1 0 0,-1 6 0 0 0,-3 6 49 0 0,-2 1 0 0 0,-10 17 0 0 0,4-6-35 0 0,-32 73 122 0 0,20-39-59 0 0,6-8 44 0 0,14-37-88 0 0,-11 25 1 0 0,10-21 10 0 0,-2 2 95 0 0,8-22-149 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,9 10 74 0 0,-6-3-46 0 0,48 69 195 0 0,-46-69-178 0 0,-2 2 1 0 0,1-2 0 0 0,0 2 0 0 0,0-2-1 0 0,-2 1 1 0 0,0 2 0 0 0,1-2 0 0 0,-1 0-1 0 0,-1 2 1 0 0,2 12 0 0 0,-4-19-32 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 2 0 0 0,-1-2 1 0 0,-2 4-1 0 0,-1 1 43 0 0,1 0 0 0 0,-2 0 1 0 0,-7 8-1 0 0,2-6-29 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-21 9 0 0 0,17-6 29 0 0,11-7-41 0 0,1-1 0 0 0,-1 1 0 0 0,-8 1 0 0 0,1 3 25 0 0,12-6-24 0 0,-2-9-2673 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1509.79">2047 602 16280 0 0,'-34'18'57'0'0,"-24"15"202"0"0,50-27-232 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-7 9 0 0 0,-1 4 69 0 0,1 2-1 0 0,0 0 0 0 0,1 0 0 0 0,-18 44 0 0 0,18-34 24 0 0,2 2 0 0 0,1 0 0 0 0,-6 38 0 0 0,14-62-95 0 0,1 2 0 0 0,0-1 0 0 0,0 1 0 0 0,2 13 0 0 0,-1-24-18 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 1 0 0 0,0-2 1 0 0,1 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,2 1 1 0 0,26 6 51 0 0,-20-6-23 0 0,2 1-17 0 0,-2-1 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,2-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,17-6 0 0 0,-2-2 33 0 0,1-2 1 0 0,40-28 0 0 0,-52 31-22 0 0,1-1-1 0 0,-1-1 1 0 0,0 1 0 0 0,-1-2 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-2 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 1-1 0 0,3-22 1 0 0,-3 14 66 0 0,-1 1-1 0 0,-1-2 1 0 0,1-34 0 0 0,-5 52-74 0 0,0-1 1 0 0,0 2 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-1-2 1 0 0,0 2 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-5-6-1 0 0,6 10 16 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-4 1 0 0 0,4-1 12 0 0,-1 1 0 0 0,0 0-1 0 0,2 1 1 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 2 0 0 0,0-2 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,-1 8 0 0 0,3-8-25 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 8 0 0 0,2 3-2737 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7426.2">2480 763 15376 0 0,'0'0'698'0'0,"2"6"-107"0"0,1 0-475 0 0,-3-4-10 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 5 1 0 0,1 24 871 0 0,-2-20-824 0 0,1-8-71 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-3 4-1 0 0,-7 26 566 0 0,-3-4-358 0 0,-33 53 0 0 0,18-38-253 0 0,-1 2 185 0 0,-2-1-1 0 0,-43 46 1 0 0,-27 41 169 0 0,83-107-347 0 0,-20 33 242 0 0,33-51-249 0 0,2 2 0 0 0,0-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-3 16 0 0 0,5-10 18 0 0,2-15-50 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,2 0 22 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,5-1 0 0 0,-2-1-10 0 0,17-6-739 0 0,-17 7-1441 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8085.02">3300 1 14672 0 0,'-2'0'21'0'0,"-13"6"398"0"0,6-2-238 0 0,-19 10 189 0 0,0 1 0 0 0,0 0 1 0 0,-33 26-1 0 0,47-29-296 0 0,1-1 1 0 0,0 1-1 0 0,0 2 0 0 0,2-2 1 0 0,0 3-1 0 0,-1-2 0 0 0,-14 30 1 0 0,-37 81 373 0 0,48-90-173 0 0,-12 34 0 0 0,25-63-209 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,0-2 0 0 0,0 1 1 0 0,0 0-1 0 0,3 9 0 0 0,-3-12-41 0 0,1-1-1 0 0,0 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,2-1 0 0 0,2 0 28 0 0,1 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,8-5 0 0 0,3-5 46 0 0,0-1-1 0 0,-2 1 1 0 0,1-3-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,-2 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-3-1 1 0 0,0 1-1 0 0,15-47 1 0 0,-9 19-12 0 0,-7 16 84 0 0,3 0 1 0 0,-1 1 0 0 0,27-50-1 0 0,-38 81 82 0 0,-6 16-33 0 0,-38 164 71 0 0,16-63-236 0 0,11-54 55 0 0,-11 54-29 0 0,-18 232 321 0 0,40-296-359 0 0,1-16 86 0 0,4 1 1 0 0,0-1-1 0 0,5 72 0 0 0,-3-101-112 0 0,-1-4 10 0 0,0 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,4 5 0 0 0,-2-8-25 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8431.52">3764 328 16687 0 0,'0'2'20'0'0,"-1"-1"50"0"0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 2 1 0 0,0-2 0 0 0,-1 1-1 0 0,-2 2 44 0 0,4-4-112 0 0,-17 20 967 0 0,16-20-932 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,-7-1-2436 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8759.18">3673 1014 15680 0 0,'0'0'0'0'0,"1"-3"-8"0"0,3-3 0 0 0,1-6 8 0 0,4-1 0 0 0,1-3-248 0 0,0-5 8 0 0,-1-5 240 0 0,-5-2 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9092.22">4329 279 14064 0 0,'0'0'432'0'0,"-6"7"832"0"0,-35 52 657 0 0,27-39-1660 0 0,0 0 0 0 0,-13 28 1 0 0,12-20-125 0 0,2 1-1 0 0,2 2 1 0 0,1-1 0 0 0,0 1-1 0 0,3 0 1 0 0,0 0 0 0 0,1 2 0 0 0,-1 37-1 0 0,4-31-51 0 0,1-17 144 0 0,1-1 0 0 0,2 36 0 0 0,0-49-189 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,1-2 0 0 0,6 10-1 0 0,-8-13-15 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 1 1 0 0,1 0 0 0 0,4-2 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 1 0 0 0,0-1-1 0 0,1-1 1 0 0,5-8-1 0 0,0-3 19 0 0,0-1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,13-36 1 0 0,-3 3-16 0 0,27-90 127 0 0,-38 114-128 0 0,-3 1 0 0 0,0 0 0 0 0,3-39-1 0 0,-8 58-22 0 0,2-58 47 0 0,-2 58-40 0 0,-1 1 0 0 0,0-2 0 0 0,1 2 0 0 0,-2-1 1 0 0,-3-12-1 0 0,4 18 2 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-4-2-1 0 0,6 4-7 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-2 4 0 0 0,-13 5 57 0 0,12-5 10 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9427.79">4970 326 14064 0 0,'-26'64'78'0'0,"-11"34"194"0"0,26-64 302 0 0,5-15-402 0 0,-7 32 0 0 0,-5 71 209 0 0,16-102-300 0 0,1 1 1 0 0,1-1 0 0 0,4 41 0 0 0,-2-49 35 0 0,0-2 0 0 0,7 19 0 0 0,-8-23-64 0 0,2-1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,2 1 1 0 0,0-2-1 0 0,0 1 1 0 0,4 3-1 0 0,-6-5-8 0 0,1-1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,3 1 0 0 0,29 3 97 0 0,-27-4-22 0 0,-4 0-97 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,8-4 0 0 0,-7 1 3 0 0,2 2 1 0 0,-1-1-1 0 0,0-1 0 0 0,-2 1 1 0 0,2-2-1 0 0,-1 1 1 0 0,4-6-1 0 0,3-9 40 0 0,-1 0 1 0 0,-1-1-1 0 0,13-36 1 0 0,-18 47-50 0 0,15-47 167 0 0,19-96 1 0 0,-36 139-163 0 0,0-1 0 0 0,-1-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,-5-17 0 0 0,4 22 16 0 0,1 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-11-6 0 0 0,13 11-4 0 0,1-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,2 2 1 0 0,-2-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-7 3 0 0 0,3-2 25 0 0,1 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 2-1 0 0,0-1 0 0 0,-8 10 0 0 0,13-12-22 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,1 0 0 0 0,-5 6 0 0 0,2 7-2624 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9758.42">5196 1272 15880 0 0,'-7'20'16'0'0,"-9"25"379"0"0,-31 61 1 0 0,41-94-326 0 0,-1 1-1 0 0,0-1 1 0 0,-1-1 0 0 0,0 1 0 0 0,-2-2 0 0 0,1 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,-16 10 0 0 0,23-17-36 0 0,-1 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-4 0 0 0 0,6-1-84 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">238 246 15072 0 0,'-15'1'143'0'0,"0"1"0"0"0,0 0 1 0 0,1 2-1 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 3 0 0 0,-12 8 1 0 0,22-14-88 0 0,0 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 2-1 0 0,0-2 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 9 0 0 0,3-4-16 0 0,0-1 1 0 0,0-1 0 0 0,1 2-1 0 0,-1-2 1 0 0,2 2 0 0 0,-1-1 0 0 0,1-1-1 0 0,0 1 1 0 0,2 0 0 0 0,-2-1-1 0 0,6 10 1 0 0,42 99 343 0 0,9 17 43 0 0,-33-78-346 0 0,67 126 612 0 0,-82-163-620 0 0,7 12 168 0 0,-1 2 0 0 0,25 56 0 0 0,-41-83-216 0 0,1 0 0 0 0,-2 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0-1-1 0 0,-1 2 1 0 0,0-1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-5 8 1 0 0,3-7 18 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-2-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,-9 3 1 0 0,0-2 12 0 0,0 0-1 0 0,0-2 1 0 0,0 1 0 0 0,-1-2 0 0 0,1 0 0 0 0,0-2 0 0 0,0 0-1 0 0,-17-4 1 0 0,17 1 14 0 0,0 0-1 0 0,-1-1 0 0 0,-27-15 1 0 0,41 19-63 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 2 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2-5-1 0 0,2 3 15 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-6 0 0 0,2-1 26 0 0,0-2 0 0 0,0 2 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,9-11 0 0 0,65-88 135 0 0,-53 80-81 0 0,-4-1 0 0 0,33-56-1 0 0,63-180 275 0 0,-96 216-321 0 0,-6 17 58 0 0,-5 11-38 0 0,0-1 0 0 0,6-28 0 0 0,-14 46-40 0 0,0-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-3-10 0 0 0,3 15-17 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 2 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,-4 0 66 0 0,-3-1 0 0 0,-9-1 0 0 0,-78-10 178 0 0,95 14-271 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,-1 1 0 0 0,2 1 0 0 0,-3 1 0 0 0,-5 3-2848 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="334.59">847 695 18991 0 0,'6'5'1256'0'0,"6"-8"1220"0"0,-10 0-2284 0 0,-2 3-174 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1-2-1 0 0,-1 2 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,0-3 37 0 0,-5-4 173 0 0,6 8-223 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2 0 0 0,-1-2 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-5 6-2996 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="662.14">733 1268 15472 0 0,'0'0'0'0'0,"0"-2"0"0"0,0 0 0 0 0,0 0 216 0 0,0-1 8 0 0,0 1-224 0 0,0-1 0 0 0,0-1 264 0 0,0-2-9 0 0,0-7-255 0 0,0-8 0 0 0,0-9 0 0 0,0-6 0 0 0,0 1 0 0 0,0 3 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1000.97">1289 408 15072 0 0,'14'-6'141'0'0,"17"-3"0"0"0,-19 7 46 0 0,-2-1 0 0 0,0-2 0 0 0,16-5 0 0 0,-20 6-6 0 0,1 0 0 0 0,0 0 0 0 0,2 2 0 0 0,-2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,15-1 0 0 0,-19 2-157 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,2 2-1 0 0,-2-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 2-1 0 0,0-2 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,2 2 1 0 0,-1-2-1 0 0,0 1 1 0 0,0-1-1 0 0,1 5 0 0 0,-1-3-10 0 0,0 2-1 0 0,0-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-2 1 0 0,-1 0-1 0 0,-1 6 0 0 0,-3 6 49 0 0,-2 1 0 0 0,-11 17 0 0 0,5-6-35 0 0,-32 73 122 0 0,19-39-59 0 0,7-8 44 0 0,14-37-88 0 0,-11 25 1 0 0,10-21 10 0 0,-2 2 95 0 0,8-22-149 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,9 10 74 0 0,-6-3-46 0 0,49 69 195 0 0,-47-69-178 0 0,-2 2 1 0 0,1-2 0 0 0,0 2 0 0 0,0-2-1 0 0,-2 1 1 0 0,0 2 0 0 0,1-2 0 0 0,-1 0-1 0 0,-1 2 1 0 0,2 12 0 0 0,-4-19-32 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 2 0 0 0,-1-2 1 0 0,-2 4-1 0 0,-1 1 43 0 0,1 0 0 0 0,-2 0 1 0 0,-7 8-1 0 0,1-6-29 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-22 9 0 0 0,18-6 29 0 0,11-7-41 0 0,1-1 0 0 0,-1 1 0 0 0,-8 1 0 0 0,1 3 25 0 0,12-6-24 0 0,-2-9-2673 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1509.79">2073 602 16280 0 0,'-35'18'57'0'0,"-24"15"202"0"0,51-27-232 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-7 9 0 0 0,-1 4 69 0 0,0 2-1 0 0,1 0 0 0 0,1 0 0 0 0,-18 44 0 0 0,18-34 24 0 0,1 2 0 0 0,2 0 0 0 0,-6 38 0 0 0,14-62-95 0 0,1 2 0 0 0,0-1 0 0 0,0 1 0 0 0,2 13 0 0 0,-1-24-18 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 1 0 0 0,0-2 1 0 0,1 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,2 1 1 0 0,27 6 51 0 0,-21-6-23 0 0,2 1-17 0 0,-2-1 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,17-6 0 0 0,-1-2 33 0 0,0-2 1 0 0,41-28 0 0 0,-53 31-22 0 0,1-1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-2 0 0 0,-2-1-1 0 0,0 1 1 0 0,0-2 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,0 1-1 0 0,3-22 1 0 0,-3 14 66 0 0,-1 1-1 0 0,-1-2 1 0 0,1-34 0 0 0,-5 52-74 0 0,0-1 1 0 0,0 2 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-1-2 1 0 0,0 2 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-5-6-1 0 0,6 10 16 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,0 0 0 0 0,-3 1 0 0 0,4-1 12 0 0,-1 1 0 0 0,0 0-1 0 0,2 1 1 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 2 0 0 0,0-2 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,0 8 0 0 0,3-8-25 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 8 0 0 0,2 3-2737 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7426.2">2511 763 15376 0 0,'0'0'698'0'0,"2"6"-107"0"0,1 0-475 0 0,-3-4-10 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 5 1 0 0,1 24 871 0 0,-2-20-824 0 0,1-8-71 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-3 4-1 0 0,-7 26 566 0 0,-3-4-358 0 0,-34 53 0 0 0,19-38-253 0 0,-1 2 185 0 0,-3-1-1 0 0,-43 46 1 0 0,-27 41 169 0 0,84-107-347 0 0,-21 33 242 0 0,34-51-249 0 0,2 2 0 0 0,0-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-3 16 0 0 0,5-10 18 0 0,2-15-50 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,2 0 22 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,5-1 0 0 0,-2-1-10 0 0,18-6-739 0 0,-18 7-1441 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8085.02">3341 1 14672 0 0,'-2'0'21'0'0,"-13"6"398"0"0,6-2-238 0 0,-19 10 189 0 0,-1 1 0 0 0,1 0 1 0 0,-34 26-1 0 0,48-29-296 0 0,1-1 1 0 0,0 1-1 0 0,-1 2 0 0 0,3-2 1 0 0,0 3-1 0 0,-1-2 0 0 0,-14 30 1 0 0,-38 81 373 0 0,49-90-173 0 0,-13 34 0 0 0,26-63-209 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,0-2 0 0 0,0 1 1 0 0,0 0-1 0 0,3 9 0 0 0,-3-12-41 0 0,1-1-1 0 0,0 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,2-1 0 0 0,2 0 28 0 0,1 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,3-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,8-5 0 0 0,4-5 46 0 0,-1-1-1 0 0,-2 1 1 0 0,1-3-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1-2 1 0 0,-2 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-2-1 1 0 0,-1 1-1 0 0,15-47 1 0 0,-9 19-12 0 0,-7 16 84 0 0,3 0 1 0 0,0 1 0 0 0,26-50-1 0 0,-38 81 82 0 0,-6 16-33 0 0,-39 164 71 0 0,17-63-236 0 0,11-54 55 0 0,-11 54-29 0 0,-19 232 321 0 0,41-296-359 0 0,1-16 86 0 0,4 1 1 0 0,0-1-1 0 0,5 72 0 0 0,-3-101-112 0 0,-1-4 10 0 0,0 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,4 5 0 0 0,-2-8-25 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8431.52">3811 328 16687 0 0,'0'2'20'0'0,"-1"-1"50"0"0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 2 1 0 0,0-2 0 0 0,-1 1-1 0 0,-2 2 44 0 0,4-4-112 0 0,-17 20 967 0 0,16-20-932 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,-7-1-2436 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8759.18">3719 1014 15680 0 0,'0'0'0'0'0,"1"-3"-8"0"0,3-3 0 0 0,1-6 8 0 0,4-1 0 0 0,1-3-248 0 0,0-5 8 0 0,0-5 240 0 0,-6-2 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9092.22">4383 279 14064 0 0,'0'0'432'0'0,"-6"7"832"0"0,-35 52 657 0 0,26-39-1660 0 0,1 0 0 0 0,-13 28 1 0 0,12-20-125 0 0,2 1-1 0 0,1 2 1 0 0,2-1 0 0 0,0 1-1 0 0,3 0 1 0 0,0 0 0 0 0,1 2 0 0 0,-1 37-1 0 0,4-31-51 0 0,1-17 144 0 0,1-1 0 0 0,2 36 0 0 0,0-49-189 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,1-2 0 0 0,6 10-1 0 0,-8-13-15 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 1 1 0 0,1 0 0 0 0,4-2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 1 0 0 0,0-1-1 0 0,1-1 1 0 0,6-8-1 0 0,-1-3 19 0 0,0-1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,13-36 1 0 0,-2 3-16 0 0,26-90 127 0 0,-38 114-128 0 0,-3 1 0 0 0,0 0 0 0 0,4-39-1 0 0,-9 58-22 0 0,2-58 47 0 0,-2 58-40 0 0,-1 1 0 0 0,0-2 0 0 0,1 2 0 0 0,-2-1 1 0 0,-4-12-1 0 0,5 18 2 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-4-2-1 0 0,6 4-7 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-2 4 0 0 0,-14 5 57 0 0,13-5 10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9427.79">5032 326 14064 0 0,'-26'64'78'0'0,"-12"34"194"0"0,27-64 302 0 0,5-15-402 0 0,-7 32 0 0 0,-5 71 209 0 0,16-102-300 0 0,1 1 1 0 0,1-1 0 0 0,4 41 0 0 0,-2-49 35 0 0,0-2 0 0 0,7 19 0 0 0,-8-23-64 0 0,2-1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,2 1 1 0 0,0-2-1 0 0,0 1 1 0 0,4 3-1 0 0,-6-5-8 0 0,1-1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,2-1 0 0 0,2 1 0 0 0,29 3 97 0 0,-27-4-22 0 0,-4 0-97 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,8-4 0 0 0,-7 1 3 0 0,2 2 1 0 0,-1-1-1 0 0,0-1 0 0 0,-2 1 1 0 0,2-2-1 0 0,-1 1 1 0 0,4-6-1 0 0,3-9 40 0 0,0 0 1 0 0,-2-1-1 0 0,13-36 1 0 0,-18 47-50 0 0,15-47 167 0 0,20-96 1 0 0,-37 139-163 0 0,0-1 0 0 0,-1-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,-5-17 0 0 0,4 22 16 0 0,1 1 1 0 0,-2 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-11-6 0 0 0,12 11-4 0 0,2-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,2 2 1 0 0,-2-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-8 3 0 0 0,4-2 25 0 0,1 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 2-1 0 0,0-1 0 0 0,-9 10 0 0 0,14-12-22 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,1 0 0 0 0,-5 6 0 0 0,2 7-2624 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9758.42">5261 1272 15880 0 0,'-7'20'16'0'0,"-9"25"379"0"0,-32 61 1 0 0,42-94-326 0 0,-1 1-1 0 0,0-1 1 0 0,-1-1 0 0 0,0 1 0 0 0,-2-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,-16 10 0 0 0,23-17-36 0 0,-1 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-5 0 0 0 0,7-1-84 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -5094,10 +5992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C341"/>
+  <dimension ref="A1:G341"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5490,7 +6388,7 @@
         <v>1.1696553591276402</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7.1428571428571397E-2</v>
       </c>
@@ -5502,7 +6400,7 @@
         <v>0.98961282862244926</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
@@ -5514,7 +6412,7 @@
         <v>1.3119411599999999</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0</v>
       </c>
@@ -5525,8 +6423,14 @@
         <f t="shared" si="0"/>
         <v>1.3119411599999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3.7037037037037E-2</v>
       </c>
@@ -5537,8 +6441,18 @@
         <f t="shared" si="0"/>
         <v>1.1391451019067214</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>-3</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <f>E36*F36</f>
+        <v>-54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.68965517241379304</v>
       </c>
@@ -5549,8 +6463,18 @@
         <f t="shared" si="0"/>
         <v>9.531911005945283E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>-2</v>
+      </c>
+      <c r="F37">
+        <v>34</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37:G42" si="1">E37*F37</f>
+        <v>-68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.30769230769230699</v>
       </c>
@@ -5561,8 +6485,18 @@
         <f t="shared" si="0"/>
         <v>0.24664212094674709</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>-1</v>
+      </c>
+      <c r="F38">
+        <v>67</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>-67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.54545454545454497</v>
       </c>
@@ -5573,8 +6507,18 @@
         <f t="shared" si="0"/>
         <v>2.2004628099163024E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>194</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -5585,8 +6529,18 @@
         <f t="shared" si="0"/>
         <v>1.3119411599999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>15</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -5597,8 +6551,18 @@
         <f t="shared" si="0"/>
         <v>1.3119411599999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.17647058823529399</v>
       </c>
@@ -5609,8 +6573,18 @@
         <f t="shared" si="0"/>
         <v>0.59801108543252646</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.55555555555555503</v>
       </c>
@@ -5621,8 +6595,16 @@
         <f t="shared" si="0"/>
         <v>6.7542234567895211E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f>SUM(F36:F42)</f>
+        <v>339</v>
+      </c>
+      <c r="G43">
+        <f>SUM(G36:G42)/F43</f>
+        <v>-0.4336283185840708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7.1428571428571397E-2</v>
       </c>
@@ -5634,7 +6616,7 @@
         <v>0.98961282862244926</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.61538461538461497</v>
       </c>
@@ -5646,7 +6628,7 @@
         <v>2.3146111479289674E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.81818181818181801</v>
       </c>
@@ -5658,7 +6640,7 @@
         <v>0.33609425132231335</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -5670,7 +6652,7 @@
         <v>0.9275616099999997</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.73333333333333295</v>
       </c>
@@ -5906,7 +6888,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="1">(2.1085*A67 - 1.1454)^2</f>
+        <f t="shared" ref="C67:C130" si="2">(2.1085*A67 - 1.1454)^2</f>
         <v>0.54930722329639825</v>
       </c>
     </row>
@@ -5918,7 +6900,7 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -5930,7 +6912,7 @@
         <v>-1</v>
       </c>
       <c r="C69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.80522118698962086</v>
       </c>
     </row>
@@ -5942,7 +6924,7 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -5954,7 +6936,7 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.31327030891975494</v>
       </c>
     </row>
@@ -5966,7 +6948,7 @@
         <v>-3</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.54361604678459996</v>
       </c>
     </row>
@@ -5978,7 +6960,7 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37415650027777697</v>
       </c>
     </row>
@@ -5990,7 +6972,7 @@
         <v>-3</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98961282862244926</v>
       </c>
     </row>
@@ -6002,7 +6984,7 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98961282862244926</v>
       </c>
     </row>
@@ -6014,7 +6996,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16665302204985974</v>
       </c>
     </row>
@@ -6026,7 +7008,7 @@
         <v>2</v>
       </c>
       <c r="C77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26957410529085779</v>
       </c>
     </row>
@@ -6038,7 +7020,7 @@
         <v>1</v>
       </c>
       <c r="C78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -6050,7 +7032,7 @@
         <v>-2</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.63040953361111352</v>
       </c>
     </row>
@@ -6062,7 +7044,7 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.10590323854938394</v>
       </c>
     </row>
@@ -6074,7 +7056,7 @@
         <v>-2</v>
       </c>
       <c r="C81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.31327030891975494</v>
       </c>
     </row>
@@ -6086,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6363183268698486E-2</v>
       </c>
     </row>
@@ -6098,7 +7080,7 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7738737777776961E-2</v>
       </c>
     </row>
@@ -6110,7 +7092,7 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6122,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4810512347448988</v>
       </c>
     </row>
@@ -6134,7 +7116,7 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -6146,7 +7128,7 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0485560771604863E-2</v>
       </c>
     </row>
@@ -6158,7 +7140,7 @@
         <v>-2</v>
       </c>
       <c r="C88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6170,7 +7152,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -6182,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.65292864159999997</v>
       </c>
     </row>
@@ -6194,7 +7176,7 @@
         <v>-1</v>
       </c>
       <c r="C91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -6206,7 +7188,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43404784668639262</v>
       </c>
     </row>
@@ -6218,7 +7200,7 @@
         <v>-2</v>
       </c>
       <c r="C93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -6230,7 +7212,7 @@
         <v>-1</v>
       </c>
       <c r="C94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -6242,7 +7224,7 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -6254,7 +7236,7 @@
         <v>0</v>
       </c>
       <c r="C96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.13008387938775459</v>
       </c>
     </row>
@@ -6266,7 +7248,7 @@
         <v>-3</v>
       </c>
       <c r="C97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -6278,7 +7260,7 @@
         <v>-1</v>
       </c>
       <c r="C98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.80522118698962086</v>
       </c>
     </row>
@@ -6290,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1609803205536337</v>
       </c>
     </row>
@@ -6302,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8446516122449589E-2</v>
       </c>
     </row>
@@ -6314,7 +7296,7 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24664212094674709</v>
       </c>
     </row>
@@ -6326,7 +7308,7 @@
         <v>0</v>
       </c>
       <c r="C102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -6338,7 +7320,7 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66014464290816111</v>
       </c>
     </row>
@@ -6350,7 +7332,7 @@
         <v>-1</v>
       </c>
       <c r="C104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -6362,7 +7344,7 @@
         <v>-1</v>
       </c>
       <c r="C105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -6374,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="C106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.10261437294896029</v>
       </c>
     </row>
@@ -6386,7 +7368,7 @@
         <v>-2</v>
       </c>
       <c r="C107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6398,7 +7380,7 @@
         <v>0</v>
       </c>
       <c r="C108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.6716753739610047E-3</v>
       </c>
     </row>
@@ -6410,7 +7392,7 @@
         <v>3</v>
       </c>
       <c r="C109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.46507853444444253</v>
       </c>
     </row>
@@ -6422,7 +7404,7 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8446516122449589E-2</v>
       </c>
     </row>
@@ -6434,7 +7416,7 @@
         <v>3</v>
       </c>
       <c r="C111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -6446,7 +7428,7 @@
         <v>-1</v>
       </c>
       <c r="C112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4810512347448988</v>
       </c>
     </row>
@@ -6458,7 +7440,7 @@
         <v>0</v>
       </c>
       <c r="C113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11184908455621385</v>
       </c>
     </row>
@@ -6470,7 +7452,7 @@
         <v>0</v>
       </c>
       <c r="C114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -6482,7 +7464,7 @@
         <v>0</v>
       </c>
       <c r="C115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -6494,7 +7476,7 @@
         <v>0</v>
       </c>
       <c r="C116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.13585432024930899</v>
       </c>
     </row>
@@ -6506,7 +7488,7 @@
         <v>-1</v>
       </c>
       <c r="C117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3384261234568351E-2</v>
       </c>
     </row>
@@ -6518,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1204000000000021E-2</v>
       </c>
     </row>
@@ -6530,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3384261234568351E-2</v>
       </c>
     </row>
@@ -6542,7 +7524,7 @@
         <v>0</v>
       </c>
       <c r="C120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32530430752066292</v>
       </c>
     </row>
@@ -6554,7 +7536,7 @@
         <v>0</v>
       </c>
       <c r="C121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1609803205536337</v>
       </c>
     </row>
@@ -6566,7 +7548,7 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8362255983378948E-2</v>
       </c>
     </row>
@@ -6578,7 +7560,7 @@
         <v>-2</v>
       </c>
       <c r="C123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6590,7 +7572,7 @@
         <v>0</v>
       </c>
       <c r="C124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -6602,7 +7584,7 @@
         <v>0</v>
       </c>
       <c r="C125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19586525444444514</v>
       </c>
     </row>
@@ -6614,7 +7596,7 @@
         <v>-1</v>
       </c>
       <c r="C126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6626,7 +7608,7 @@
         <v>-2</v>
       </c>
       <c r="C127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6638,7 +7620,7 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1103386663327031</v>
       </c>
     </row>
@@ -6650,7 +7632,7 @@
         <v>-1</v>
       </c>
       <c r="C129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1015742853099177</v>
       </c>
     </row>
@@ -6662,7 +7644,7 @@
         <v>0</v>
       </c>
       <c r="C130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37415650027777697</v>
       </c>
     </row>
@@ -6674,7 +7656,7 @@
         <v>0</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C194" si="2">(2.1085*A131 - 1.1454)^2</f>
+        <f t="shared" ref="C131:C194" si="3">(2.1085*A131 - 1.1454)^2</f>
         <v>0.16665302204985974</v>
       </c>
     </row>
@@ -6686,7 +7668,7 @@
         <v>2</v>
       </c>
       <c r="C132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.21807251795847712</v>
       </c>
     </row>
@@ -6698,7 +7680,7 @@
         <v>0</v>
       </c>
       <c r="C133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9726070156249951E-2</v>
       </c>
     </row>
@@ -6710,7 +7692,7 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1609803205536337</v>
       </c>
     </row>
@@ -6722,7 +7704,7 @@
         <v>0</v>
       </c>
       <c r="C135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6716753739610047E-3</v>
       </c>
     </row>
@@ -6734,7 +7716,7 @@
         <v>-1</v>
       </c>
       <c r="C136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.71264952020408467</v>
       </c>
     </row>
@@ -6746,7 +7728,7 @@
         <v>-1</v>
       </c>
       <c r="C137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -6758,7 +7740,7 @@
         <v>0</v>
       </c>
       <c r="C138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.43809269877550949</v>
       </c>
     </row>
@@ -6770,7 +7752,7 @@
         <v>0</v>
       </c>
       <c r="C139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -6782,7 +7764,7 @@
         <v>-2</v>
       </c>
       <c r="C140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6794,7 +7776,7 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -6806,7 +7788,7 @@
         <v>-1</v>
       </c>
       <c r="C142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6818,7 +7800,7 @@
         <v>-1</v>
       </c>
       <c r="C143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.34872754573407239</v>
       </c>
     </row>
@@ -6830,7 +7812,7 @@
         <v>-1</v>
       </c>
       <c r="C144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -6842,7 +7824,7 @@
         <v>0</v>
       </c>
       <c r="C145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.34872754573407239</v>
       </c>
     </row>
@@ -6854,7 +7836,7 @@
         <v>0</v>
       </c>
       <c r="C146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -6866,7 +7848,7 @@
         <v>-1</v>
       </c>
       <c r="C147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6878,7 +7860,7 @@
         <v>0</v>
       </c>
       <c r="C148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -6890,7 +7872,7 @@
         <v>-1</v>
       </c>
       <c r="C149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -6902,7 +7884,7 @@
         <v>-2</v>
       </c>
       <c r="C150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6914,7 +7896,7 @@
         <v>0</v>
       </c>
       <c r="C151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16066736111111043</v>
       </c>
     </row>
@@ -6926,7 +7908,7 @@
         <v>-1</v>
       </c>
       <c r="C152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6938,7 +7920,7 @@
         <v>0</v>
       </c>
       <c r="C153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -6950,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="C154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -6962,7 +7944,7 @@
         <v>0</v>
       </c>
       <c r="C155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13585432024930899</v>
       </c>
     </row>
@@ -6974,7 +7956,7 @@
         <v>0</v>
       </c>
       <c r="C156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -6986,7 +7968,7 @@
         <v>-3</v>
       </c>
       <c r="C157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0700378027977842</v>
       </c>
     </row>
@@ -6998,7 +7980,7 @@
         <v>0</v>
       </c>
       <c r="C158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -7010,7 +7992,7 @@
         <v>0</v>
       </c>
       <c r="C159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6716753739610047E-3</v>
       </c>
     </row>
@@ -7022,7 +8004,7 @@
         <v>-2</v>
       </c>
       <c r="C160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7034,7 +8016,7 @@
         <v>0</v>
       </c>
       <c r="C161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3541777777781162E-4</v>
       </c>
     </row>
@@ -7046,7 +8028,7 @@
         <v>0</v>
       </c>
       <c r="C162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -7058,7 +8040,7 @@
         <v>0</v>
       </c>
       <c r="C163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -7070,7 +8052,7 @@
         <v>-2</v>
       </c>
       <c r="C164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.7738737777776961E-2</v>
       </c>
     </row>
@@ -7082,7 +8064,7 @@
         <v>0</v>
       </c>
       <c r="C165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.72684623889660827</v>
       </c>
     </row>
@@ -7094,7 +8076,7 @@
         <v>0</v>
       </c>
       <c r="C166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7106,7 +8088,7 @@
         <v>0</v>
       </c>
       <c r="C167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13585432024930899</v>
       </c>
     </row>
@@ -7118,7 +8100,7 @@
         <v>1</v>
       </c>
       <c r="C168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.46507853444444253</v>
       </c>
     </row>
@@ -7130,7 +8112,7 @@
         <v>0</v>
       </c>
       <c r="C169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.22997577440443318</v>
       </c>
     </row>
@@ -7142,7 +8124,7 @@
         <v>0</v>
       </c>
       <c r="C170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.60638046132325429</v>
       </c>
     </row>
@@ -7154,7 +8136,7 @@
         <v>0</v>
       </c>
       <c r="C171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.87338370249999997</v>
       </c>
     </row>
@@ -7166,7 +8148,7 @@
         <v>0</v>
       </c>
       <c r="C172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -7178,7 +8160,7 @@
         <v>0</v>
       </c>
       <c r="C173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -7190,7 +8172,7 @@
         <v>0</v>
       </c>
       <c r="C174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.37415650027777697</v>
       </c>
     </row>
@@ -7202,7 +8184,7 @@
         <v>0</v>
       </c>
       <c r="C175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -7214,7 +8196,7 @@
         <v>0</v>
       </c>
       <c r="C176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13008387938775459</v>
       </c>
     </row>
@@ -7226,7 +8208,7 @@
         <v>0</v>
       </c>
       <c r="C177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.4127004132652262E-2</v>
       </c>
     </row>
@@ -7238,7 +8220,7 @@
         <v>0</v>
       </c>
       <c r="C178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.46507853444444253</v>
       </c>
     </row>
@@ -7250,7 +8232,7 @@
         <v>0</v>
       </c>
       <c r="C179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7262,7 +8244,7 @@
         <v>0</v>
       </c>
       <c r="C180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7274,7 +8256,7 @@
         <v>-2</v>
       </c>
       <c r="C181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7286,7 +8268,7 @@
         <v>0</v>
       </c>
       <c r="C182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -7298,7 +8280,7 @@
         <v>0</v>
       </c>
       <c r="C183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -7310,7 +8292,7 @@
         <v>0</v>
       </c>
       <c r="C184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0700378027977842</v>
       </c>
     </row>
@@ -7322,7 +8304,7 @@
         <v>0</v>
       </c>
       <c r="C185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.8562248016528612E-2</v>
       </c>
     </row>
@@ -7334,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="C186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.56258437816406248</v>
       </c>
     </row>
@@ -7346,7 +8328,7 @@
         <v>-2</v>
       </c>
       <c r="C187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -7358,7 +8340,7 @@
         <v>0</v>
       </c>
       <c r="C188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3541777777781162E-4</v>
       </c>
     </row>
@@ -7370,7 +8352,7 @@
         <v>0</v>
       </c>
       <c r="C189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6363183268698486E-2</v>
       </c>
     </row>
@@ -7382,7 +8364,7 @@
         <v>-1</v>
       </c>
       <c r="C190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7394,7 +8376,7 @@
         <v>0</v>
       </c>
       <c r="C191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -7406,7 +8388,7 @@
         <v>0</v>
       </c>
       <c r="C192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16066736111111043</v>
       </c>
     </row>
@@ -7418,7 +8400,7 @@
         <v>0</v>
       </c>
       <c r="C193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4701807091412677E-2</v>
       </c>
     </row>
@@ -7430,7 +8412,7 @@
         <v>-1</v>
       </c>
       <c r="C194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.29481797224489964</v>
       </c>
     </row>
@@ -7442,7 +8424,7 @@
         <v>0</v>
       </c>
       <c r="C195">
-        <f t="shared" ref="C195:C258" si="3">(2.1085*A195 - 1.1454)^2</f>
+        <f t="shared" ref="C195:C258" si="4">(2.1085*A195 - 1.1454)^2</f>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7454,7 +8436,7 @@
         <v>-2</v>
       </c>
       <c r="C196">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0573209126234571</v>
       </c>
     </row>
@@ -7466,7 +8448,7 @@
         <v>-3</v>
       </c>
       <c r="C197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7478,7 +8460,7 @@
         <v>-1</v>
       </c>
       <c r="C198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7490,7 +8472,7 @@
         <v>-1</v>
       </c>
       <c r="C199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -7502,7 +8484,7 @@
         <v>0</v>
       </c>
       <c r="C200">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.90957837033057842</v>
       </c>
     </row>
@@ -7514,7 +8496,7 @@
         <v>-2</v>
       </c>
       <c r="C201">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.4810512347448988</v>
       </c>
     </row>
@@ -7526,7 +8508,7 @@
         <v>0</v>
       </c>
       <c r="C202">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.19586525444444514</v>
       </c>
     </row>
@@ -7538,7 +8520,7 @@
         <v>0</v>
       </c>
       <c r="C203">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.4127004132652262E-2</v>
       </c>
     </row>
@@ -7550,7 +8532,7 @@
         <v>-1</v>
       </c>
       <c r="C204">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -7562,7 +8544,7 @@
         <v>0</v>
       </c>
       <c r="C205">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8446516122449589E-2</v>
       </c>
     </row>
@@ -7574,7 +8556,7 @@
         <v>1</v>
       </c>
       <c r="C206">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -7586,7 +8568,7 @@
         <v>0</v>
       </c>
       <c r="C207">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7598,7 +8580,7 @@
         <v>0</v>
       </c>
       <c r="C208">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16066736111111043</v>
       </c>
     </row>
@@ -7610,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="C209">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7622,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="C210">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.16665302204985974</v>
       </c>
     </row>
@@ -7634,7 +8616,7 @@
         <v>0</v>
       </c>
       <c r="C211">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8453241890581341E-2</v>
       </c>
     </row>
@@ -7646,7 +8628,7 @@
         <v>0</v>
       </c>
       <c r="C212">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -7658,7 +8640,7 @@
         <v>0</v>
       </c>
       <c r="C213">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.22997577440443318</v>
       </c>
     </row>
@@ -7670,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="C214">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -7682,7 +8664,7 @@
         <v>1</v>
       </c>
       <c r="C215">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.60801345272211482</v>
       </c>
     </row>
@@ -7694,7 +8676,7 @@
         <v>-3</v>
       </c>
       <c r="C216">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0700378027977842</v>
       </c>
     </row>
@@ -7706,7 +8688,7 @@
         <v>0</v>
       </c>
       <c r="C217">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.7375875600000034E-2</v>
       </c>
     </row>
@@ -7718,7 +8700,7 @@
         <v>-1</v>
       </c>
       <c r="C218">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -7730,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="C219">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -7742,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="C220">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8446516122449589E-2</v>
       </c>
     </row>
@@ -7754,7 +8736,7 @@
         <v>0</v>
       </c>
       <c r="C221">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -7766,7 +8748,7 @@
         <v>-2</v>
       </c>
       <c r="C222">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7778,7 +8760,7 @@
         <v>-2</v>
       </c>
       <c r="C223">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -7790,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="C224">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.77763737640625008</v>
       </c>
     </row>
@@ -7802,7 +8784,7 @@
         <v>0</v>
       </c>
       <c r="C225">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.54930722329639825</v>
       </c>
     </row>
@@ -7814,7 +8796,7 @@
         <v>-1</v>
       </c>
       <c r="C226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -7826,7 +8808,7 @@
         <v>0</v>
       </c>
       <c r="C227">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.8803832485206591E-2</v>
       </c>
     </row>
@@ -7838,7 +8820,7 @@
         <v>1</v>
       </c>
       <c r="C228">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.46507853444444253</v>
       </c>
     </row>
@@ -7850,7 +8832,7 @@
         <v>0</v>
       </c>
       <c r="C229">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7862,7 +8844,7 @@
         <v>0</v>
       </c>
       <c r="C230">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8446516122449589E-2</v>
       </c>
     </row>
@@ -7874,7 +8856,7 @@
         <v>0</v>
       </c>
       <c r="C231">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9698342226562511E-2</v>
       </c>
     </row>
@@ -7886,7 +8868,7 @@
         <v>-1</v>
       </c>
       <c r="C232">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7898,7 +8880,7 @@
         <v>-1</v>
       </c>
       <c r="C233">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.67406626177515094</v>
       </c>
     </row>
@@ -7910,7 +8892,7 @@
         <v>0</v>
       </c>
       <c r="C234">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -7922,7 +8904,7 @@
         <v>-1</v>
       </c>
       <c r="C235">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7934,7 +8916,7 @@
         <v>0</v>
       </c>
       <c r="C236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -7946,7 +8928,7 @@
         <v>-2</v>
       </c>
       <c r="C237">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0096900277777781</v>
       </c>
     </row>
@@ -7958,7 +8940,7 @@
         <v>0</v>
       </c>
       <c r="C238">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7738737777776961E-2</v>
       </c>
     </row>
@@ -7970,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="C239">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3459427128028135E-2</v>
       </c>
     </row>
@@ -7982,7 +8964,7 @@
         <v>0</v>
       </c>
       <c r="C240">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.7927511730103088E-2</v>
       </c>
     </row>
@@ -7994,7 +8976,7 @@
         <v>0</v>
       </c>
       <c r="C241">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -8006,7 +8988,7 @@
         <v>-1</v>
       </c>
       <c r="C242">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -8018,7 +9000,7 @@
         <v>0</v>
       </c>
       <c r="C243">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.63040953361111352</v>
       </c>
     </row>
@@ -8030,7 +9012,7 @@
         <v>-3</v>
       </c>
       <c r="C244">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8042,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="C245">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.9698342226562511E-2</v>
       </c>
     </row>
@@ -8054,7 +9036,7 @@
         <v>-3</v>
       </c>
       <c r="C246">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.47201081831758052</v>
       </c>
     </row>
@@ -8066,7 +9048,7 @@
         <v>-1</v>
       </c>
       <c r="C247">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8078,7 +9060,7 @@
         <v>0</v>
       </c>
       <c r="C248">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2718608310249781E-3</v>
       </c>
     </row>
@@ -8090,7 +9072,7 @@
         <v>-1</v>
       </c>
       <c r="C249">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8102,7 +9084,7 @@
         <v>-2</v>
       </c>
       <c r="C250">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8114,7 +9096,7 @@
         <v>-3</v>
       </c>
       <c r="C251">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8126,7 +9108,7 @@
         <v>3</v>
       </c>
       <c r="C252">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.39712550570636912</v>
       </c>
     </row>
@@ -8138,7 +9120,7 @@
         <v>-1</v>
       </c>
       <c r="C253">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -8150,7 +9132,7 @@
         <v>-1</v>
       </c>
       <c r="C254">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -8162,7 +9144,7 @@
         <v>0</v>
       </c>
       <c r="C255">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -8174,7 +9156,7 @@
         <v>0</v>
       </c>
       <c r="C256">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0700378027977842</v>
       </c>
     </row>
@@ -8186,7 +9168,7 @@
         <v>0</v>
       </c>
       <c r="C257">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.29481797224489964</v>
       </c>
     </row>
@@ -8198,7 +9180,7 @@
         <v>0</v>
       </c>
       <c r="C258">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -8210,7 +9192,7 @@
         <v>-1</v>
       </c>
       <c r="C259">
-        <f t="shared" ref="C259:C322" si="4">(2.1085*A259 - 1.1454)^2</f>
+        <f t="shared" ref="C259:C322" si="5">(2.1085*A259 - 1.1454)^2</f>
         <v>4.3384261234568351E-2</v>
       </c>
     </row>
@@ -8222,7 +9204,7 @@
         <v>0</v>
       </c>
       <c r="C260">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14243495336419704</v>
       </c>
     </row>
@@ -8234,7 +9216,7 @@
         <v>-3</v>
       </c>
       <c r="C261">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8246,7 +9228,7 @@
         <v>0</v>
       </c>
       <c r="C262">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -8258,7 +9240,7 @@
         <v>0</v>
       </c>
       <c r="C263">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.23667616878906256</v>
       </c>
     </row>
@@ -8270,7 +9252,7 @@
         <v>0</v>
       </c>
       <c r="C264">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.19586525444444514</v>
       </c>
     </row>
@@ -8282,7 +9264,7 @@
         <v>0</v>
       </c>
       <c r="C265">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.22997577440443318</v>
       </c>
     </row>
@@ -8294,7 +9276,7 @@
         <v>0</v>
       </c>
       <c r="C266">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12582095765624998</v>
       </c>
     </row>
@@ -8306,7 +9288,7 @@
         <v>0</v>
       </c>
       <c r="C267">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1204000000000021E-2</v>
       </c>
     </row>
@@ -8318,7 +9300,7 @@
         <v>-2</v>
       </c>
       <c r="C268">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.38226397562500003</v>
       </c>
     </row>
@@ -8330,7 +9312,7 @@
         <v>0</v>
       </c>
       <c r="C269">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7542234567895211E-4</v>
       </c>
     </row>
@@ -8342,7 +9324,7 @@
         <v>-2</v>
       </c>
       <c r="C270">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.66012203991689822</v>
       </c>
     </row>
@@ -8354,7 +9336,7 @@
         <v>-1</v>
       </c>
       <c r="C271">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.96669736621301783</v>
       </c>
     </row>
@@ -8366,7 +9348,7 @@
         <v>-2</v>
       </c>
       <c r="C272">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10590323854938394</v>
       </c>
     </row>
@@ -8378,7 +9360,7 @@
         <v>-1</v>
       </c>
       <c r="C273">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -8390,7 +9372,7 @@
         <v>0</v>
       </c>
       <c r="C274">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14339303438016637</v>
       </c>
     </row>
@@ -8402,7 +9384,7 @@
         <v>0</v>
       </c>
       <c r="C275">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0107982248523018E-4</v>
       </c>
     </row>
@@ -8414,7 +9396,7 @@
         <v>0</v>
       </c>
       <c r="C276">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -8426,7 +9408,7 @@
         <v>1</v>
       </c>
       <c r="C277">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.9275616099999997</v>
       </c>
     </row>
@@ -8438,7 +9420,7 @@
         <v>0</v>
       </c>
       <c r="C278">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -8450,7 +9432,7 @@
         <v>-1</v>
       </c>
       <c r="C279">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8462,7 +9444,7 @@
         <v>0</v>
       </c>
       <c r="C280">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16066736111111043</v>
       </c>
     </row>
@@ -8474,7 +9456,7 @@
         <v>0</v>
       </c>
       <c r="C281">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -8486,7 +9468,7 @@
         <v>-1</v>
       </c>
       <c r="C282">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34872754573407239</v>
       </c>
     </row>
@@ -8498,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="C283">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.19586525444444514</v>
       </c>
     </row>
@@ -8510,7 +9492,7 @@
         <v>-2</v>
       </c>
       <c r="C284">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1391451019067214</v>
       </c>
     </row>
@@ -8522,7 +9504,7 @@
         <v>0</v>
       </c>
       <c r="C285">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -8534,7 +9516,7 @@
         <v>-2</v>
       </c>
       <c r="C286">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8546,7 +9528,7 @@
         <v>0</v>
       </c>
       <c r="C287">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15394973270408191</v>
       </c>
     </row>
@@ -8558,7 +9540,7 @@
         <v>-2</v>
       </c>
       <c r="C288">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8570,7 +9552,7 @@
         <v>0</v>
       </c>
       <c r="C289">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3083225000000118E-3</v>
       </c>
     </row>
@@ -8582,7 +9564,7 @@
         <v>0</v>
       </c>
       <c r="C290">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -8594,7 +9576,7 @@
         <v>-3</v>
       </c>
       <c r="C291">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8606,7 +9588,7 @@
         <v>0</v>
       </c>
       <c r="C292">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.67656108444444296</v>
       </c>
     </row>
@@ -8618,7 +9600,7 @@
         <v>-1</v>
       </c>
       <c r="C293">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8630,7 +9612,7 @@
         <v>0</v>
       </c>
       <c r="C294">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -8642,7 +9624,7 @@
         <v>0</v>
       </c>
       <c r="C295">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -8654,7 +9636,7 @@
         <v>0</v>
       </c>
       <c r="C296">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0700378027977842</v>
       </c>
     </row>
@@ -8666,7 +9648,7 @@
         <v>-1</v>
       </c>
       <c r="C297">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.63040953361111352</v>
       </c>
     </row>
@@ -8678,7 +9660,7 @@
         <v>0</v>
       </c>
       <c r="C298">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1103386663327031</v>
       </c>
     </row>
@@ -8690,7 +9672,7 @@
         <v>-1</v>
       </c>
       <c r="C299">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0573209126234571</v>
       </c>
     </row>
@@ -8702,7 +9684,7 @@
         <v>-1</v>
       </c>
       <c r="C300">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15394973270408191</v>
       </c>
     </row>
@@ -8714,7 +9696,7 @@
         <v>-1</v>
       </c>
       <c r="C301">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34872754573407239</v>
       </c>
     </row>
@@ -8726,7 +9708,7 @@
         <v>0</v>
       </c>
       <c r="C302">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16066736111111043</v>
       </c>
     </row>
@@ -8738,7 +9720,7 @@
         <v>0</v>
       </c>
       <c r="C303">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.39712550570636912</v>
       </c>
     </row>
@@ -8750,7 +9732,7 @@
         <v>0</v>
       </c>
       <c r="C304">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6060721111111573E-2</v>
       </c>
     </row>
@@ -8762,7 +9744,7 @@
         <v>0</v>
       </c>
       <c r="C305">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.16665302204985974</v>
       </c>
     </row>
@@ -8774,7 +9756,7 @@
         <v>0</v>
       </c>
       <c r="C306">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14243495336419704</v>
       </c>
     </row>
@@ -8786,7 +9768,7 @@
         <v>0</v>
       </c>
       <c r="C307">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.77763737640625008</v>
       </c>
     </row>
@@ -8798,7 +9780,7 @@
         <v>0</v>
       </c>
       <c r="C308">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3187393264745728E-2</v>
       </c>
     </row>
@@ -8810,7 +9792,7 @@
         <v>0</v>
       </c>
       <c r="C309">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -8822,7 +9804,7 @@
         <v>0</v>
       </c>
       <c r="C310">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.31327030891975494</v>
       </c>
     </row>
@@ -8834,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="C311">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34004448444444607</v>
       </c>
     </row>
@@ -8846,7 +9828,7 @@
         <v>-1</v>
       </c>
       <c r="C312">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -8858,7 +9840,7 @@
         <v>0</v>
       </c>
       <c r="C313">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.72611925806093947</v>
       </c>
     </row>
@@ -8870,7 +9852,7 @@
         <v>0</v>
       </c>
       <c r="C314">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.22997577440443318</v>
       </c>
     </row>
@@ -8882,7 +9864,7 @@
         <v>0</v>
       </c>
       <c r="C315">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1502363462604406E-2</v>
       </c>
     </row>
@@ -8894,7 +9876,7 @@
         <v>0</v>
       </c>
       <c r="C316">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -8906,7 +9888,7 @@
         <v>0</v>
       </c>
       <c r="C317">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.27589065221453418</v>
       </c>
     </row>
@@ -8918,7 +9900,7 @@
         <v>0</v>
       </c>
       <c r="C318">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.51128388404844094</v>
       </c>
     </row>
@@ -8930,7 +9912,7 @@
         <v>0</v>
       </c>
       <c r="C319">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.13585432024930899</v>
       </c>
     </row>
@@ -8942,7 +9924,7 @@
         <v>0</v>
       </c>
       <c r="C320">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3541777777781162E-4</v>
       </c>
     </row>
@@ -8954,7 +9936,7 @@
         <v>-2</v>
       </c>
       <c r="C321">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0573209126234571</v>
       </c>
     </row>
@@ -8966,7 +9948,7 @@
         <v>0</v>
       </c>
       <c r="C322">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.42156757384083271</v>
       </c>
     </row>
@@ -8978,7 +9960,7 @@
         <v>-1</v>
       </c>
       <c r="C323">
-        <f t="shared" ref="C323:C340" si="5">(2.1085*A323 - 1.1454)^2</f>
+        <f t="shared" ref="C323:C340" si="6">(2.1085*A323 - 1.1454)^2</f>
         <v>0.94030192840277793</v>
       </c>
     </row>
@@ -8990,7 +9972,7 @@
         <v>-2</v>
       </c>
       <c r="C324">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -9002,7 +9984,7 @@
         <v>0</v>
       </c>
       <c r="C325">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4965600082645085E-2</v>
       </c>
     </row>
@@ -9014,7 +9996,7 @@
         <v>-3</v>
       </c>
       <c r="C326">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98961282862244926</v>
       </c>
     </row>
@@ -9026,7 +10008,7 @@
         <v>-1</v>
       </c>
       <c r="C327">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.96669736621301783</v>
       </c>
     </row>
@@ -9038,7 +10020,7 @@
         <v>0</v>
       </c>
       <c r="C328">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -9050,7 +10032,7 @@
         <v>-1</v>
       </c>
       <c r="C329">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.74695687111111242</v>
       </c>
     </row>
@@ -9062,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="C330">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.32530430752066292</v>
       </c>
     </row>
@@ -9074,7 +10056,7 @@
         <v>-1</v>
       </c>
       <c r="C331">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49210963423822918</v>
       </c>
     </row>
@@ -9086,7 +10068,7 @@
         <v>0</v>
       </c>
       <c r="C332">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.33609425132231335</v>
       </c>
     </row>
@@ -9098,7 +10080,7 @@
         <v>0</v>
       </c>
       <c r="C333">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.52374169000000004</v>
       </c>
     </row>
@@ -9110,7 +10092,7 @@
         <v>0</v>
       </c>
       <c r="C334">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.32530430752066292</v>
       </c>
     </row>
@@ -9122,7 +10104,7 @@
         <v>0</v>
       </c>
       <c r="C335">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.85276476277008628</v>
       </c>
     </row>
@@ -9134,7 +10116,7 @@
         <v>0</v>
       </c>
       <c r="C336">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.1204000000000021E-2</v>
       </c>
     </row>
@@ -9146,7 +10128,7 @@
         <v>0</v>
       </c>
       <c r="C337">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.15058633024793336</v>
       </c>
     </row>
@@ -9158,7 +10140,7 @@
         <v>0</v>
       </c>
       <c r="C338">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4701807091412677E-2</v>
       </c>
     </row>
@@ -9170,7 +10152,7 @@
         <v>-1</v>
       </c>
       <c r="C339">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3119411599999999</v>
       </c>
     </row>
@@ -9182,7 +10164,7 @@
         <v>0</v>
       </c>
       <c r="C340">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.32530430752066292</v>
       </c>
     </row>

</xml_diff>